<commit_message>
Locked frames not overlaying regular symbols
</commit_message>
<xml_diff>
--- a/Math/Valiant-1.0Math.xlsx
+++ b/Math/Valiant-1.0Math.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="17655" windowHeight="10920" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="17655" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="30" r:id="rId1"/>
@@ -970,7 +970,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1007,6 +1007,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1023,7 +1029,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1055,6 +1061,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1393,7 +1400,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ59"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="T5" sqref="T5:X16"/>
     </sheetView>
   </sheetViews>
@@ -1425,30 +1432,30 @@
       </c>
       <c r="AC1">
         <f>MIN($AA$14)</f>
-        <v>15.186020502038712</v>
+        <v>5.9308497139790699</v>
       </c>
       <c r="AG1">
         <v>1</v>
       </c>
       <c r="AH1" s="6">
         <f t="shared" ref="AH1:AL1" si="0">3*L5</f>
-        <v>2.5482625482625481</v>
+        <v>1.5271966527196654</v>
       </c>
       <c r="AI1" s="6">
         <f t="shared" si="0"/>
-        <v>0.34526854219948849</v>
+        <v>8.9955022488755615E-2</v>
       </c>
       <c r="AJ1" s="6">
         <f t="shared" si="0"/>
-        <v>0.35386631716906947</v>
+        <v>9.7402597402597393E-2</v>
       </c>
       <c r="AK1" s="6">
         <f t="shared" si="0"/>
-        <v>7.0422535211267595E-2</v>
+        <v>0.5</v>
       </c>
       <c r="AL1" s="6">
         <f t="shared" si="0"/>
-        <v>9.6774193548387094E-2</v>
+        <v>0.34682080924855491</v>
       </c>
       <c r="AM1">
         <v>1</v>
@@ -1582,30 +1589,30 @@
       </c>
       <c r="AF4" s="22">
         <f>PRODUCT(AH4:AL4)</f>
-        <v>-0.54993596408774281</v>
+        <v>-0.14142686856023637</v>
       </c>
       <c r="AG4" s="5">
         <v>1</v>
       </c>
       <c r="AH4" s="6">
         <f>1-AH1</f>
-        <v>-1.5482625482625481</v>
+        <v>-0.52719665271966543</v>
       </c>
       <c r="AI4" s="6">
         <f t="shared" ref="AI4:AL4" si="1">1-AI1</f>
-        <v>0.65473145780051145</v>
+        <v>0.91004497751124436</v>
       </c>
       <c r="AJ4" s="6">
         <f t="shared" si="1"/>
-        <v>0.64613368283093053</v>
+        <v>0.90259740259740262</v>
       </c>
       <c r="AK4" s="6">
         <f t="shared" si="1"/>
-        <v>0.92957746478873238</v>
+        <v>0.5</v>
       </c>
       <c r="AL4" s="6">
         <f t="shared" si="1"/>
-        <v>0.90322580645161288</v>
+        <v>0.65317919075144504</v>
       </c>
       <c r="AM4" s="5">
         <v>1</v>
@@ -1622,67 +1629,67 @@
         <v>0</v>
       </c>
       <c r="E5" s="26">
-        <f>-SUM(E6:E$16,-E$18)</f>
-        <v>660</v>
+        <v>365</v>
       </c>
       <c r="F5">
-        <v>90</v>
+        <f>E6</f>
+        <v>20</v>
       </c>
       <c r="G5">
         <f>F5</f>
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K5" s="12">
         <v>0</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ref="L5:P7" si="2">E5/E$17</f>
-        <v>0.84942084942084939</v>
+        <v>0.50906555090655514</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="2"/>
-        <v>0.11508951406649616</v>
+        <v>2.9985007496251874E-2</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" si="2"/>
-        <v>0.11795543905635648</v>
+        <v>3.2467532467532464E-2</v>
       </c>
       <c r="O5" s="6">
         <f t="shared" si="2"/>
-        <v>2.3474178403755867E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="2"/>
-        <v>3.2258064516129031E-2</v>
+        <v>0.11560693641618497</v>
       </c>
       <c r="Q5" s="7">
         <v>0</v>
       </c>
       <c r="T5" t="str">
-        <f t="shared" ref="T5:T16" si="3">"x"&amp;E5&amp;" "&amp;$D5</f>
-        <v>x660 0</v>
+        <f t="shared" ref="T5:T15" si="3">"x"&amp;E5&amp;" "&amp;$D5</f>
+        <v>x365 0</v>
       </c>
       <c r="U5" t="str">
         <f t="shared" ref="U5:U15" si="4">"x"&amp;F5&amp;" "&amp;$D5</f>
-        <v>x90 0</v>
+        <v>x20 0</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" ref="V5:V15" si="5">"x"&amp;G5&amp;" "&amp;$D5</f>
-        <v>x90 0</v>
+        <v>x20 0</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" ref="W5:W15" si="6">"x"&amp;H5&amp;" "&amp;$D5</f>
-        <v>x5 0</v>
+        <v>x30 0</v>
       </c>
       <c r="X5" t="str">
-        <f t="shared" ref="X5:X16" si="7">"x"&amp;I5&amp;" "&amp;$D5</f>
-        <v>x5 0</v>
+        <f t="shared" ref="X5:X15" si="7">"x"&amp;I5&amp;" "&amp;$D5</f>
+        <v>x20 0</v>
       </c>
       <c r="Z5" s="12" t="s">
         <v>48</v>
@@ -1692,35 +1699,35 @@
       </c>
       <c r="AC5" t="b">
         <f>$AA$6&gt;=0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5">
         <v>1</v>
       </c>
       <c r="AF5" s="22">
         <f>SUM(AH5:AL5)</f>
-        <v>0.21336072434215875</v>
+        <v>0.16392667965755889</v>
       </c>
       <c r="AG5" s="5"/>
       <c r="AH5" s="6">
         <f>PRODUCT($AG4:AG4,AI4:$AM4)*AH1</f>
-        <v>0.90513151196486363</v>
+        <v>0.40968894463877997</v>
       </c>
       <c r="AI5" s="6">
         <f>PRODUCT($AG4:AH4,AJ4:$AM4)*AI1</f>
-        <v>-0.29000529356189569</v>
+        <v>-1.3979591620451702E-2</v>
       </c>
       <c r="AJ5" s="6">
         <f>PRODUCT($AG4:AI4,AK4:$AM4)*AJ1</f>
-        <v>-0.30118196816164416</v>
+        <v>-1.526189229067299E-2</v>
       </c>
       <c r="AK5" s="6">
         <f>PRODUCT($AG4:AJ4,AL4:$AM4)*AK1</f>
-        <v>-4.1661815461192638E-2</v>
+        <v>-0.14142686856023637</v>
       </c>
       <c r="AL5" s="6">
         <f>PRODUCT($AG4:AK4,AM4:$AM4)*AL1</f>
-        <v>-5.8921710437972445E-2</v>
+        <v>-7.5093912509860028E-2</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -1735,20 +1742,22 @@
         <v>1</v>
       </c>
       <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6" s="26">
+        <f>E5</f>
+        <v>365</v>
+      </c>
+      <c r="G6">
+        <f>F7</f>
+        <v>20</v>
+      </c>
+      <c r="H6">
         <v>30</v>
       </c>
-      <c r="F6" s="26">
-        <f>-SUM(F7:F$16,-F$18,F5)</f>
-        <v>606</v>
-      </c>
-      <c r="G6">
+      <c r="I6">
+        <f>H5</f>
         <v>30</v>
-      </c>
-      <c r="H6">
-        <v>10</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
       </c>
       <c r="K6" s="12">
         <f t="shared" ref="K6:K16" si="9">K5+1</f>
@@ -1756,53 +1765,53 @@
       </c>
       <c r="L6" s="6">
         <f t="shared" si="2"/>
-        <v>3.8610038610038609E-2</v>
+        <v>2.7894002789400279E-2</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="2"/>
-        <v>0.77493606138107418</v>
+        <v>0.54722638680659674</v>
       </c>
       <c r="N6" s="6">
         <f t="shared" si="2"/>
-        <v>3.9318479685452164E-2</v>
+        <v>3.2467532467532464E-2</v>
       </c>
       <c r="O6" s="6">
         <f t="shared" si="2"/>
-        <v>4.6948356807511735E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="2"/>
-        <v>6.4516129032258063E-2</v>
+        <v>0.17341040462427745</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
       </c>
       <c r="T6" t="str">
         <f t="shared" si="3"/>
-        <v>x30 1</v>
+        <v>x20 1</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" si="4"/>
-        <v>x606 1</v>
+        <v>x365 1</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" si="5"/>
-        <v>x30 1</v>
+        <v>x20 1</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="6"/>
-        <v>x10 1</v>
+        <v>x30 1</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" si="7"/>
-        <v>x10 1</v>
+        <v>x30 1</v>
       </c>
       <c r="Z6" s="12" t="s">
         <v>50</v>
       </c>
       <c r="AA6" s="5">
         <f>B9-(AA4-AA5)</f>
-        <v>5.5292903943725236</v>
+        <v>-8.3103936219211541</v>
       </c>
       <c r="AB6" s="19" t="s">
         <v>37</v>
@@ -1816,48 +1825,48 @@
       </c>
       <c r="AF6" s="23">
         <f>SUM(AH6:AQ6)</f>
-        <v>0.86715676061505731</v>
+        <v>0.59055993369993409</v>
       </c>
       <c r="AG6" s="5"/>
       <c r="AH6" s="6">
         <f>PRODUCT(AH4:AJ4)*PRODUCT(AK1,AL1)</f>
-        <v>-4.4637659422706397E-3</v>
+        <v>-7.5093912509860028E-2</v>
       </c>
       <c r="AI6" s="6">
         <f>PRODUCT(AH4:AI4,AK4)*PRODUCT(AJ1,AL1)</f>
-        <v>-3.2269496588747594E-2</v>
+        <v>-8.1036596233661894E-3</v>
       </c>
       <c r="AJ6" s="6">
         <f>PRODUCT(AH4:AI4,AL4)*PRODUCT(AJ1,AK1)</f>
-        <v>-2.2816815769821523E-2</v>
+        <v>-1.526189229067299E-2</v>
       </c>
       <c r="AK6" s="6">
         <f>PRODUCT(AH4,AJ4,AK4)*PRODUCT(AI1,AL1)</f>
-        <v>-3.107199573877454E-2</v>
+        <v>-7.422792010859311E-3</v>
       </c>
       <c r="AL6" s="6">
         <f>PRODUCT(AH4,AJ4,AL4)*PRODUCT(AI1,AK1)</f>
-        <v>-2.1970097997113306E-2</v>
+        <v>-1.3979591620451702E-2</v>
       </c>
       <c r="AM6" s="6">
         <f>PRODUCT(AH4,AK4,AL4)*PRODUCT(AI1,AJ1)</f>
-        <v>-0.15882642852274206</v>
+        <v>-1.5085890237897519E-3</v>
       </c>
       <c r="AN6" s="6">
         <f>PRODUCT(AI4,AJ4,AK4)*PRODUCT(AH1,AL1)</f>
-        <v>9.6978376281949677E-2</v>
+        <v>0.21753395290554689</v>
       </c>
       <c r="AO6" s="6">
         <f>PRODUCT(AI4,AJ4,AL4)*PRODUCT(AH1,AK1)</f>
-        <v>6.8570569088247227E-2</v>
+        <v>0.40968894463877997</v>
       </c>
       <c r="AP6" s="6">
         <f>PRODUCT(AI4,AK4,AL4)*PRODUCT(AH1,AJ1)</f>
-        <v>0.49571097004160897</v>
+        <v>4.4211037191235245E-2</v>
       </c>
       <c r="AQ6" s="6">
         <f>PRODUCT(AJ4,AK4,AL4)*PRODUCT(AH1,AI1)</f>
-        <v>0.47731544576272111</v>
+        <v>4.0496436043371983E-2</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -1873,20 +1882,23 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>30</v>
+        <f>E6</f>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <f t="shared" ref="F7:F8" si="10">E7</f>
+        <v>20</v>
       </c>
       <c r="G7" s="26">
-        <f>-SUM(G8:G$16,-G$18,G$5:G6)</f>
-        <v>608</v>
+        <f>F6-1</f>
+        <v>364</v>
       </c>
       <c r="H7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <f t="shared" ref="I5:I7" si="11">H7</f>
+        <v>20</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" si="9"/>
@@ -1894,53 +1906,53 @@
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>3.8610038610038609E-2</v>
+        <v>2.7894002789400279E-2</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
-        <v>3.8363171355498722E-2</v>
+        <v>2.9985007496251874E-2</v>
       </c>
       <c r="N7" s="6">
         <f t="shared" si="2"/>
-        <v>0.79685452162516379</v>
+        <v>0.59090909090909094</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" si="2"/>
-        <v>4.6948356807511735E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
-        <v>6.4516129032258063E-2</v>
+        <v>0.11560693641618497</v>
       </c>
       <c r="Q7" s="7">
         <v>0</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="3"/>
-        <v>x30 2</v>
+        <v>x20 2</v>
       </c>
       <c r="U7" t="str">
         <f t="shared" si="4"/>
-        <v>x30 2</v>
+        <v>x20 2</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="5"/>
-        <v>x608 2</v>
+        <v>x364 2</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="6"/>
-        <v>x10 2</v>
+        <v>x20 2</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="7"/>
-        <v>x10 2</v>
+        <v>x20 2</v>
       </c>
       <c r="Z7" s="12" t="s">
         <v>51</v>
       </c>
       <c r="AA7" s="5">
         <f>(AA4+AA5)-B9</f>
-        <v>34.470709605627476</v>
+        <v>48.31039362192115</v>
       </c>
       <c r="AB7" s="19" t="s">
         <v>37</v>
@@ -1954,48 +1966,48 @@
       </c>
       <c r="AF7" s="23">
         <f>SUM(AH7:AQ7)</f>
-        <v>0.41287586078363547</v>
+        <v>0.33375290317563433</v>
       </c>
       <c r="AG7" s="5"/>
       <c r="AH7" s="6">
         <f>PRODUCT(AH1:AJ1)*PRODUCT(AK4,AL4)</f>
-        <v>0.26141008185787973</v>
+        <v>4.3701189974861858E-3</v>
       </c>
       <c r="AI7" s="6">
         <f>PRODUCT(AH1:AI1,AK1)*PRODUCT(AJ4,AL4)</f>
-        <v>3.6160261042630384E-2</v>
+        <v>4.0496436043371983E-2</v>
       </c>
       <c r="AJ7" s="6">
         <f>PRODUCT(AH1:AI1,AL1)*PRODUCT(AJ4,AK4)</f>
-        <v>5.1140940617434405E-2</v>
+        <v>2.1502532412409906E-2</v>
       </c>
       <c r="AK7" s="6">
         <f>PRODUCT(AH1,AJ1,AK1)*PRODUCT(AI4,AL4)</f>
-        <v>3.7553861366788545E-2</v>
+        <v>4.4211037191235245E-2</v>
       </c>
       <c r="AL7" s="6">
         <f>PRODUCT(AH1,AJ1,AL1)*PRODUCT(AI4,AK4)</f>
-        <v>5.3111889647315239E-2</v>
+        <v>2.3474887004195706E-2</v>
       </c>
       <c r="AM7" s="6">
         <f>PRODUCT(AH1,AK1,AL1)*PRODUCT(AI4,AJ4)</f>
-        <v>7.3468466880264888E-3</v>
+        <v>0.21753395290554689</v>
       </c>
       <c r="AN7" s="6">
         <f>PRODUCT(AI1,AJ1,AK1)*PRODUCT(AH4,AL4)</f>
-        <v>-1.203230519111682E-2</v>
+        <v>-1.5085890237897519E-3</v>
       </c>
       <c r="AO7" s="6">
         <f>PRODUCT(AI1,AJ1,AL1)*PRODUCT(AH4,AK4)</f>
-        <v>-1.7017117341722364E-2</v>
+        <v>-8.0102072059632843E-4</v>
       </c>
       <c r="AP7" s="6">
         <f>PRODUCT(AI1,AK1,AL1)*PRODUCT(AH4,AJ4)</f>
-        <v>-2.3539390711192825E-3</v>
+        <v>-7.422792010859311E-3</v>
       </c>
       <c r="AQ7" s="6">
         <f>PRODUCT(AJ1,AK1,AL1)*PRODUCT(AH4,AI4)</f>
-        <v>-2.4446588324808778E-3</v>
+        <v>-8.1036596233661894E-3</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -2009,68 +2021,68 @@
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="E8">
-        <v>17</v>
+      <c r="E8" s="27">
+        <v>250</v>
       </c>
       <c r="F8">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" s="26">
-        <f>-SUM(H9:H$16,-H$18,H$5:H7)</f>
-        <v>126</v>
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
       </c>
       <c r="I8">
-        <v>35</v>
+        <f>H9</f>
+        <v>25</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" ref="L8:L13" si="10">E8/E$17</f>
-        <v>2.1879021879021878E-2</v>
+        <f t="shared" ref="L8:L13" si="12">E8/E$17</f>
+        <v>0.34867503486750351</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" ref="M8:M13" si="11">F8/F$17</f>
-        <v>2.1739130434782608E-2</v>
+        <f t="shared" ref="M8:M13" si="13">F8/F$17</f>
+        <v>1.7991004497751123E-2</v>
       </c>
       <c r="N8" s="6">
-        <f t="shared" ref="N8:N13" si="12">G8/G$17</f>
-        <v>3.9318479685452159E-3</v>
+        <f t="shared" ref="N8:N13" si="14">G8/G$17</f>
+        <v>1.948051948051948E-2</v>
       </c>
       <c r="O8" s="6">
-        <f t="shared" ref="O8:O13" si="13">H8/H$17</f>
-        <v>0.59154929577464788</v>
+        <f t="shared" ref="O8:O13" si="15">H8/H$17</f>
+        <v>0.1111111111111111</v>
       </c>
       <c r="P8" s="6">
-        <f t="shared" ref="P8:P13" si="14">I8/I$17</f>
-        <v>0.22580645161290322</v>
+        <f t="shared" ref="P8:P13" si="16">I8/I$17</f>
+        <v>0.14450867052023122</v>
       </c>
       <c r="Q8" s="7">
         <v>0</v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="3"/>
-        <v>x17 3</v>
+        <v>x250 3</v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="4"/>
-        <v>x17 3</v>
+        <v>x12 3</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="5"/>
-        <v>x3 3</v>
+        <v>x12 3</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="6"/>
-        <v>x126 3</v>
+        <v>x20 3</v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="7"/>
-        <v>x35 3</v>
+        <v>x25 3</v>
       </c>
       <c r="AC8" t="b">
         <f>$AA$16&gt;=$AA$17</f>
@@ -2081,27 +2093,27 @@
       </c>
       <c r="AF8" s="23">
         <f>SUM(AH8:AL8)</f>
-        <v>5.4420783266876167E-2</v>
+        <v>5.086693486030229E-2</v>
       </c>
       <c r="AH8" s="24">
         <f>PRODUCT($AG1:AG1,AI1:$AM1)*AH4</f>
-        <v>-1.289175556191088E-3</v>
+        <v>-8.0102072059632843E-4</v>
       </c>
       <c r="AI8" s="24">
         <f>PRODUCT($AG1:AH1,AJ1:$AM1)*AI4</f>
-        <v>4.0236280035844873E-3</v>
+        <v>2.3474887004195706E-2</v>
       </c>
       <c r="AJ8" s="24">
         <f>PRODUCT($AG1:AI1,AK1:$AM1)*AJ4</f>
-        <v>3.8743136831389698E-3</v>
+        <v>2.1502532412409906E-2</v>
       </c>
       <c r="AK8" s="24">
         <f>PRODUCT($AG1:AJ1,AL1:$AM1)*AK4</f>
-        <v>2.8008223056201396E-2</v>
+        <v>2.3204171668068244E-3</v>
       </c>
       <c r="AL8" s="24">
         <f>PRODUCT($AG1:AK1,AM1:$AM1)*AL4</f>
-        <v>1.9803794080142399E-2</v>
+        <v>4.3701189974861858E-3</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -2110,74 +2122,75 @@
       </c>
       <c r="B9" s="5">
         <f>SUM(L22:P33)</f>
-        <v>35.529290394372524</v>
+        <v>21.689606378078846</v>
       </c>
       <c r="D9" s="12">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="E9">
-        <v>10</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="F9" s="27">
+        <v>200</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <f>G8</f>
+        <v>12</v>
       </c>
       <c r="H9">
-        <v>35</v>
-      </c>
-      <c r="I9" s="26">
-        <f>-SUM(I10:I$16,-I$18,I$5:I8)</f>
-        <v>68</v>
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <f>H10</f>
+        <v>24</v>
       </c>
       <c r="K9" s="12">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="10"/>
-        <v>1.2870012870012869E-2</v>
+        <f t="shared" si="12"/>
+        <v>1.6736401673640166E-2</v>
       </c>
       <c r="M9" s="6">
-        <f t="shared" si="11"/>
-        <v>1.278772378516624E-2</v>
+        <f t="shared" si="13"/>
+        <v>0.29985007496251875</v>
       </c>
       <c r="N9" s="6">
-        <f t="shared" si="12"/>
-        <v>3.9318479685452159E-3</v>
+        <f t="shared" si="14"/>
+        <v>1.948051948051948E-2</v>
       </c>
       <c r="O9" s="6">
-        <f t="shared" si="13"/>
-        <v>0.16431924882629109</v>
+        <f t="shared" si="15"/>
+        <v>0.1388888888888889</v>
       </c>
       <c r="P9" s="6">
-        <f t="shared" si="14"/>
-        <v>0.43870967741935485</v>
+        <f t="shared" si="16"/>
+        <v>0.13872832369942195</v>
       </c>
       <c r="Q9" s="7">
         <v>0</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="3"/>
-        <v>x10 4</v>
+        <v>x12 4</v>
       </c>
       <c r="U9" t="str">
         <f t="shared" si="4"/>
-        <v>x10 4</v>
+        <v>x200 4</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="5"/>
-        <v>x3 4</v>
+        <v>x12 4</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="6"/>
-        <v>x35 4</v>
+        <v>x25 4</v>
       </c>
       <c r="X9" t="str">
         <f t="shared" si="7"/>
-        <v>x68 4</v>
+        <v>x24 4</v>
       </c>
       <c r="Z9" s="12" t="s">
         <v>52</v>
@@ -2194,7 +2207,7 @@
       </c>
       <c r="AF9" s="23">
         <f>PRODUCT(AH1:AL1)</f>
-        <v>2.1218350800152569E-3</v>
+        <v>2.3204171668068244E-3</v>
       </c>
       <c r="AG9" s="5"/>
     </row>
@@ -2204,7 +2217,7 @@
       </c>
       <c r="B10" s="5">
         <f>100*(1-(1-SUMIF(T22:X33,"&lt;&gt;0",E22:I33)/100)^B6)</f>
-        <v>2.3388347812337895</v>
+        <v>1.2859064428135558</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -2214,66 +2227,68 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
+        <f t="shared" ref="F10:I10" si="17">E10</f>
+        <v>12</v>
+      </c>
+      <c r="G10" s="27">
+        <v>150</v>
       </c>
       <c r="H10">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="I10">
-        <v>5</v>
+        <f t="shared" si="17"/>
+        <v>24</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="10"/>
-        <v>6.4350064350064346E-3</v>
+        <f t="shared" si="12"/>
+        <v>1.6736401673640166E-2</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" si="11"/>
-        <v>6.3938618925831201E-3</v>
+        <f t="shared" si="13"/>
+        <v>1.7991004497751123E-2</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" si="12"/>
-        <v>6.55307994757536E-3</v>
+        <f t="shared" si="14"/>
+        <v>0.2435064935064935</v>
       </c>
       <c r="O10" s="6">
-        <f t="shared" si="13"/>
-        <v>2.3474178403755867E-2</v>
+        <f t="shared" si="15"/>
+        <v>0.13333333333333333</v>
       </c>
       <c r="P10" s="6">
-        <f t="shared" si="14"/>
-        <v>3.2258064516129031E-2</v>
+        <f t="shared" si="16"/>
+        <v>0.13872832369942195</v>
       </c>
       <c r="Q10" s="7">
         <v>0</v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="3"/>
-        <v>x5 5</v>
+        <v>x12 5</v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="4"/>
-        <v>x5 5</v>
+        <v>x12 5</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="5"/>
-        <v>x5 5</v>
+        <v>x150 5</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="6"/>
-        <v>x5 5</v>
+        <v>x24 5</v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="7"/>
-        <v>x5 5</v>
+        <v>x24 5</v>
       </c>
       <c r="Z10" s="12" t="s">
         <v>53</v>
@@ -2287,7 +2302,7 @@
       </c>
       <c r="AF10" s="22">
         <f>SUM(AF4:AF9)</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -2296,7 +2311,7 @@
       </c>
       <c r="B11" s="5">
         <f>1/$B$6*(1/100*SUMPRODUCT(F22:I33,U22:X33,U22:X33)-(1/100*SUMPRODUCT(F22:I33,U22:X33))^2)</f>
-        <v>7.095541396566631</v>
+        <v>7.576995615248606</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -2306,73 +2321,76 @@
         <v>6</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <f t="shared" ref="F10:I13" si="18">E11</f>
+        <v>12</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <f>F11</f>
+        <v>12</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>4</v>
+        <f t="shared" ref="H11:I11" si="19">H11</f>
+        <v>5</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="10"/>
-        <v>5.1480051480051478E-3</v>
+        <f t="shared" si="12"/>
+        <v>1.6736401673640166E-2</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" si="11"/>
-        <v>5.1150895140664966E-3</v>
+        <f t="shared" si="13"/>
+        <v>1.7991004497751123E-2</v>
       </c>
       <c r="N11" s="6">
-        <f t="shared" si="12"/>
-        <v>5.2424639580602884E-3</v>
+        <f t="shared" si="14"/>
+        <v>1.948051948051948E-2</v>
       </c>
       <c r="O11" s="6">
-        <f t="shared" si="13"/>
-        <v>1.8779342723004695E-2</v>
+        <f t="shared" si="15"/>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="P11" s="6">
-        <f t="shared" si="14"/>
-        <v>2.5806451612903226E-2</v>
+        <f t="shared" si="16"/>
+        <v>2.8901734104046242E-2</v>
       </c>
       <c r="Q11" s="7">
         <v>0</v>
       </c>
       <c r="T11" t="str">
         <f t="shared" si="3"/>
-        <v>x4 6</v>
+        <v>x12 6</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" si="4"/>
-        <v>x4 6</v>
+        <v>x12 6</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="5"/>
-        <v>x4 6</v>
+        <v>x12 6</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="6"/>
-        <v>x4 6</v>
+        <v>x5 6</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="7"/>
-        <v>x4 6</v>
+        <v>x5 6</v>
       </c>
       <c r="Z11" s="12" t="s">
         <v>54</v>
       </c>
       <c r="AA11" s="5">
         <f>B10-(AA9-AA10)</f>
-        <v>-7.6611652187662109</v>
+        <v>-8.7140935571864446</v>
       </c>
       <c r="AB11" s="19" t="s">
         <v>37</v>
@@ -2388,7 +2406,7 @@
       </c>
       <c r="B12" s="5">
         <f>SQRT(B11)</f>
-        <v>2.663745745480719</v>
+        <v>2.752634304670456</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -2398,73 +2416,76 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <f t="shared" si="18"/>
+        <v>10</v>
       </c>
       <c r="G12">
-        <v>3</v>
+        <f>F12</f>
+        <v>10</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>3</v>
+        <f t="shared" ref="H12:I12" si="20">H12</f>
+        <v>5</v>
       </c>
       <c r="K12" s="12">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="10"/>
-        <v>3.8610038610038611E-3</v>
+        <f t="shared" si="12"/>
+        <v>1.3947001394700139E-2</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="11"/>
-        <v>3.8363171355498722E-3</v>
+        <f t="shared" si="13"/>
+        <v>1.4992503748125937E-2</v>
       </c>
       <c r="N12" s="6">
-        <f t="shared" si="12"/>
-        <v>3.9318479685452159E-3</v>
+        <f t="shared" si="14"/>
+        <v>1.6233766233766232E-2</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="13"/>
-        <v>1.4084507042253521E-2</v>
+        <f t="shared" si="15"/>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="P12" s="6">
-        <f t="shared" si="14"/>
-        <v>1.935483870967742E-2</v>
+        <f t="shared" si="16"/>
+        <v>2.8901734104046242E-2</v>
       </c>
       <c r="Q12" s="7">
         <v>0</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="3"/>
-        <v>x3 7</v>
+        <v>x10 7</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="4"/>
-        <v>x3 7</v>
+        <v>x10 7</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="5"/>
-        <v>x3 7</v>
+        <v>x10 7</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="6"/>
-        <v>x3 7</v>
+        <v>x5 7</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="7"/>
-        <v>x3 7</v>
+        <v>x5 7</v>
       </c>
       <c r="Z12" s="12" t="s">
         <v>55</v>
       </c>
       <c r="AA12" s="5">
         <f>(AA9+AA10)-B10</f>
-        <v>37.661165218766207</v>
+        <v>38.714093557186445</v>
       </c>
       <c r="AB12" s="19" t="s">
         <v>37</v>
@@ -2478,11 +2499,11 @@
       </c>
       <c r="AF12" s="23">
         <f>SUM(AF13:AF15)</f>
-        <v>0.46941847913052687</v>
+        <v>0.38694025520274344</v>
       </c>
       <c r="AG12">
         <f>1/AF12</f>
-        <v>2.1302953429789016</v>
+        <v>2.5843783027331551</v>
       </c>
     </row>
     <row r="13" spans="1:43">
@@ -2494,66 +2515,69 @@
         <v>8</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <f>F13</f>
+        <v>5</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <f t="shared" si="18"/>
+        <v>5</v>
       </c>
       <c r="K13" s="12">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="10"/>
-        <v>2.5740025740025739E-3</v>
+        <f t="shared" si="12"/>
+        <v>6.9735006973500697E-3</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="11"/>
-        <v>2.5575447570332483E-3</v>
+        <f t="shared" si="13"/>
+        <v>7.4962518740629685E-3</v>
       </c>
       <c r="N13" s="6">
-        <f t="shared" si="12"/>
-        <v>2.6212319790301442E-3</v>
+        <f t="shared" si="14"/>
+        <v>4.87012987012987E-3</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="13"/>
-        <v>9.3896713615023476E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="P13" s="6">
-        <f t="shared" si="14"/>
-        <v>1.2903225806451613E-2</v>
+        <f t="shared" si="16"/>
+        <v>2.8901734104046242E-2</v>
       </c>
       <c r="Q13" s="7">
         <v>0</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="3"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="4"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="5"/>
-        <v>x2 8</v>
+        <v>x3 8</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="6"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="7"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="AC13" t="b">
         <f>$E$9=INT($E$9)</f>
@@ -2564,15 +2588,15 @@
       </c>
       <c r="AF13" s="23">
         <f>AF7</f>
-        <v>0.41287586078363547</v>
+        <v>0.33375290317563433</v>
       </c>
       <c r="AG13">
         <f>1/AF13</f>
-        <v>2.4220355195917898</v>
+        <v>2.9962286184931233</v>
       </c>
       <c r="AH13" s="5">
-        <f t="shared" ref="AH13:AH15" si="15">AF13/AF$12*100</f>
-        <v>87.954752345578385</v>
+        <f t="shared" ref="AH13:AH15" si="21">AF13/AF$12*100</f>
+        <v>86.254376144130902</v>
       </c>
     </row>
     <row r="14" spans="1:43">
@@ -2581,74 +2605,74 @@
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="E14" s="25">
-        <v>0</v>
-      </c>
-      <c r="F14" s="25">
-        <v>0</v>
-      </c>
-      <c r="G14" s="25">
-        <v>0</v>
-      </c>
-      <c r="H14" s="25">
-        <v>0</v>
-      </c>
-      <c r="I14" s="25">
-        <v>0</v>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
       </c>
       <c r="K14" s="12">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="L14" s="6">
-        <f t="shared" ref="L14:P17" si="16">E14/E$17</f>
-        <v>0</v>
+        <f t="shared" ref="L14:P17" si="22">E14/E$17</f>
+        <v>2.7894002789400278E-3</v>
       </c>
       <c r="M14" s="6">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>2.9985007496251873E-3</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>3.246753246753247E-3</v>
       </c>
       <c r="O14" s="6">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="P14" s="6">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>1.1560693641618497E-2</v>
       </c>
       <c r="Q14" s="7">
         <v>0</v>
       </c>
       <c r="T14" t="str">
         <f t="shared" si="3"/>
-        <v>x0 9</v>
+        <v>x2 9</v>
       </c>
       <c r="U14" t="str">
         <f t="shared" si="4"/>
-        <v>x0 9</v>
+        <v>x2 9</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="5"/>
-        <v>x0 9</v>
+        <v>x2 9</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="6"/>
-        <v>x0 9</v>
+        <v>x2 9</v>
       </c>
       <c r="X14" t="str">
         <f t="shared" si="7"/>
-        <v>x0 9</v>
+        <v>x2 9</v>
       </c>
       <c r="Z14" s="12" t="s">
         <v>56</v>
       </c>
       <c r="AA14" s="21">
         <f>MAX(N22:P33)-MIN(N22:P33)</f>
-        <v>15.186020502038712</v>
+        <v>5.9308497139790699</v>
       </c>
       <c r="AC14" t="b">
         <f>$E$10=INT($E$10)</f>
@@ -2659,15 +2683,15 @@
       </c>
       <c r="AF14" s="23">
         <f>AF8</f>
-        <v>5.4420783266876167E-2</v>
+        <v>5.086693486030229E-2</v>
       </c>
       <c r="AG14">
         <f>1/AF14</f>
-        <v>18.375332730807301</v>
+        <v>19.659136190264586</v>
       </c>
       <c r="AH14" s="5">
-        <f t="shared" si="15"/>
-        <v>11.593234115469041</v>
+        <f t="shared" si="21"/>
+        <v>13.145940277950599</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -2676,58 +2700,62 @@
         <v>10</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <f>ROUND(E18*4/350,0)</f>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <f t="shared" ref="F15:I15" si="23">ROUND(F18*4/350,0)</f>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <f t="shared" si="23"/>
+        <v>5</v>
       </c>
       <c r="H15">
         <v>4</v>
       </c>
       <c r="I15">
-        <v>4</v>
+        <f>ROUND(I18*4/230,0)</f>
+        <v>3</v>
       </c>
       <c r="K15" s="12">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="16"/>
-        <v>3.8610038610038611E-3</v>
+        <f t="shared" si="22"/>
+        <v>6.9735006973500697E-3</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="16"/>
-        <v>3.8363171355498722E-3</v>
+        <f t="shared" si="22"/>
+        <v>7.4962518740629685E-3</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="16"/>
-        <v>3.9318479685452159E-3</v>
+        <f t="shared" si="22"/>
+        <v>8.1168831168831161E-3</v>
       </c>
       <c r="O15" s="6">
-        <f t="shared" si="16"/>
-        <v>1.8779342723004695E-2</v>
+        <f t="shared" si="22"/>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="P15" s="6">
-        <f t="shared" si="16"/>
-        <v>2.5806451612903226E-2</v>
+        <f t="shared" si="22"/>
+        <v>1.7341040462427744E-2</v>
       </c>
       <c r="Q15" s="7">
         <v>0</v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="3"/>
-        <v>x3 10</v>
+        <v>x5 10</v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="4"/>
-        <v>x3 10</v>
+        <v>x5 10</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="5"/>
-        <v>x3 10</v>
+        <v>x5 10</v>
       </c>
       <c r="W15" t="str">
         <f t="shared" si="6"/>
@@ -2735,7 +2763,7 @@
       </c>
       <c r="X15" t="str">
         <f t="shared" si="7"/>
-        <v>x4 10</v>
+        <v>x3 10</v>
       </c>
       <c r="AC15" t="b">
         <f>$E$11=INT($E$11)</f>
@@ -2746,21 +2774,21 @@
       </c>
       <c r="AF15" s="23">
         <f>AF9</f>
-        <v>2.1218350800152569E-3</v>
+        <v>2.3204171668068244E-3</v>
       </c>
       <c r="AG15">
         <f>1/AF15</f>
-        <v>471.29016266090275</v>
+        <v>430.95699096905122</v>
       </c>
       <c r="AH15" s="5">
-        <f t="shared" si="15"/>
-        <v>0.45201353895257662</v>
+        <f t="shared" si="21"/>
+        <v>0.59968357791850968</v>
       </c>
     </row>
     <row r="16" spans="1:43">
       <c r="A16">
         <f>1-(1-4*E16/E17)^5</f>
-        <v>0.2927304858294153</v>
+        <v>0.10670621694510263</v>
       </c>
       <c r="B16" s="5"/>
       <c r="D16" s="12">
@@ -2768,73 +2796,73 @@
         <v>11</v>
       </c>
       <c r="E16">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K16" s="12">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.6731016731016731E-2</v>
+        <f t="shared" si="22"/>
+        <v>5.5788005578800556E-3</v>
       </c>
       <c r="M16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.5345268542199489E-2</v>
+        <f t="shared" si="22"/>
+        <v>5.9970014992503746E-3</v>
       </c>
       <c r="N16" s="6">
-        <f t="shared" si="16"/>
-        <v>1.5727391874180863E-2</v>
+        <f t="shared" si="22"/>
+        <v>9.74025974025974E-3</v>
       </c>
       <c r="O16" s="6">
-        <f t="shared" si="16"/>
-        <v>4.2253521126760563E-2</v>
+        <f t="shared" si="22"/>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="P16" s="6">
-        <f t="shared" si="16"/>
-        <v>5.8064516129032261E-2</v>
+        <f t="shared" si="22"/>
+        <v>5.7803468208092484E-2</v>
       </c>
       <c r="Q16" s="7">
         <v>0</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" ref="T16" si="17">"x"&amp;E16&amp;" "&amp;$D16</f>
-        <v>x13 11</v>
+        <f t="shared" ref="T16" si="24">"x"&amp;E16&amp;" "&amp;$D16</f>
+        <v>x4 11</v>
       </c>
       <c r="U16" t="str">
-        <f t="shared" ref="U16" si="18">"x"&amp;F16&amp;" "&amp;$D16</f>
-        <v>x12 11</v>
+        <f t="shared" ref="U16" si="25">"x"&amp;F16&amp;" "&amp;$D16</f>
+        <v>x4 11</v>
       </c>
       <c r="V16" t="str">
-        <f t="shared" ref="V16" si="19">"x"&amp;G16&amp;" "&amp;$D16</f>
-        <v>x12 11</v>
+        <f t="shared" ref="V16" si="26">"x"&amp;G16&amp;" "&amp;$D16</f>
+        <v>x6 11</v>
       </c>
       <c r="W16" t="str">
-        <f t="shared" ref="W16" si="20">"x"&amp;H16&amp;" "&amp;$D16</f>
-        <v>x9 11</v>
+        <f t="shared" ref="W16" si="27">"x"&amp;H16&amp;" "&amp;$D16</f>
+        <v>x10 11</v>
       </c>
       <c r="X16" t="str">
-        <f t="shared" ref="X16" si="21">"x"&amp;I16&amp;" "&amp;$D16</f>
-        <v>x9 11</v>
+        <f t="shared" ref="X16" si="28">"x"&amp;I16&amp;" "&amp;$D16</f>
+        <v>x10 11</v>
       </c>
       <c r="Z16" s="12" t="s">
         <v>58</v>
       </c>
       <c r="AA16" s="21">
         <f>MAX(E5:I16)</f>
-        <v>660</v>
+        <v>365</v>
       </c>
       <c r="AC16" t="b">
         <f>$E$12=INT($E$12)</f>
@@ -2844,47 +2872,47 @@
     <row r="17" spans="1:31">
       <c r="A17">
         <f>1/A16^3</f>
-        <v>39.865401229082131</v>
+        <v>823.05873917924941</v>
       </c>
       <c r="B17" s="5"/>
       <c r="E17" s="1">
         <f>SUM(E5:E16)</f>
-        <v>777</v>
+        <v>717</v>
       </c>
       <c r="F17" s="1">
         <f>SUM(F5:F16)</f>
-        <v>782</v>
+        <v>667</v>
       </c>
       <c r="G17" s="1">
         <f>SUM(G5:G16)</f>
-        <v>763</v>
+        <v>616</v>
       </c>
       <c r="H17" s="1">
         <f>SUM(H5:H16)</f>
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="I17" s="1">
         <f>SUM($I$5:I16)</f>
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="N17" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="O17" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="P17" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="Z17" s="12" t="s">
@@ -2892,7 +2920,7 @@
       </c>
       <c r="AA17" s="21">
         <f>MIN(E5:I16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AC17" t="b">
         <f>$E$13=INT($E$13)</f>
@@ -2905,19 +2933,22 @@
     <row r="18" spans="1:31">
       <c r="B18" s="5"/>
       <c r="E18">
-        <v>777</v>
+        <v>400</v>
       </c>
       <c r="F18">
-        <v>782</v>
+        <f t="shared" ref="F18:I18" si="29">E18</f>
+        <v>400</v>
       </c>
       <c r="G18">
-        <v>763</v>
+        <f t="shared" si="29"/>
+        <v>400</v>
       </c>
       <c r="H18">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="I18">
-        <v>155</v>
+        <f>H18</f>
+        <v>200</v>
       </c>
       <c r="AC18" t="b">
         <f>$E$14=INT($E$14)</f>
@@ -2930,7 +2961,7 @@
     <row r="19" spans="1:31">
       <c r="AA19">
         <f>_xlfn.STDEV.S(N22:P33)</f>
-        <v>3.5209675902763093</v>
+        <v>1.4216902316312305</v>
       </c>
       <c r="AC19" t="b">
         <f>$E$15=INT($E$15)</f>
@@ -2950,7 +2981,7 @@
       </c>
       <c r="AA20" s="21">
         <f>SUMSQ(N22:P33)-SUM(N22:P33)*SUM(N22:P33)</f>
-        <v>-793.36329347305127</v>
+        <v>-386.62916513106154</v>
       </c>
       <c r="AC20" t="b">
         <f>$E$16=INT($E$16)</f>
@@ -3005,7 +3036,7 @@
       </c>
       <c r="AA21">
         <f>_xlfn.VAR.S(N22:P33)</f>
-        <v>12.397212771776159</v>
+        <v>2.0212031147156622</v>
       </c>
       <c r="AC21" t="b">
         <f>$F$5=INT($F$5)</f>
@@ -3019,45 +3050,45 @@
       </c>
       <c r="E22" s="5">
         <f>L5*(1-M5)*100</f>
-        <v>75.166141662305336</v>
+        <v>49.380121654653848</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" ref="F22:I24" si="22">E22/(1-M5)*M5*(1-N5)</f>
-        <v>8.6228175980231541</v>
+        <f t="shared" ref="F22:I24" si="30">E22/(1-M5)*M5*(1-N5)</f>
+        <v>1.4768739088587535</v>
       </c>
       <c r="G22" s="5">
-        <f t="shared" si="22"/>
-        <v>1.1260570037809363</v>
+        <f t="shared" si="30"/>
+        <v>4.1299605952425995E-2</v>
       </c>
       <c r="H22" s="9">
-        <f t="shared" si="22"/>
-        <v>2.6195494815003172E-2</v>
+        <f t="shared" si="30"/>
+        <v>7.3050170066140761E-3</v>
       </c>
       <c r="I22" s="9">
-        <f t="shared" si="22"/>
-        <v>8.7318316050010575E-4</v>
+        <f t="shared" si="30"/>
+        <v>9.5490418387112104E-4</v>
       </c>
       <c r="K22" s="12">
         <v>0</v>
       </c>
       <c r="L22" s="16">
-        <f t="shared" ref="L22:L33" si="23">E22*T22</f>
+        <f t="shared" ref="L22:L33" si="31">E22*T22</f>
         <v>0</v>
       </c>
       <c r="M22" s="16">
-        <f t="shared" ref="M22:M33" si="24">F22*U22</f>
+        <f t="shared" ref="M22:M33" si="32">F22*U22</f>
         <v>0</v>
       </c>
       <c r="N22" s="16">
-        <f t="shared" ref="N22:N33" si="25">G22*V22</f>
+        <f t="shared" ref="N22:N33" si="33">G22*V22</f>
         <v>0</v>
       </c>
       <c r="O22" s="16">
-        <f t="shared" ref="O22:O33" si="26">H22*W22</f>
+        <f t="shared" ref="O22:O33" si="34">H22*W22</f>
         <v>0</v>
       </c>
       <c r="P22" s="16">
-        <f t="shared" ref="P22:P33" si="27">I22*X22</f>
+        <f t="shared" ref="P22:P33" si="35">I22*X22</f>
         <v>0</v>
       </c>
       <c r="S22" s="12">
@@ -3080,7 +3111,7 @@
       </c>
       <c r="AA22" s="21">
         <f>SUM(N22:P33)</f>
-        <v>35.529290394372524</v>
+        <v>21.689606378078846</v>
       </c>
       <c r="AC22" t="b">
         <f>$F$6=INT($F$6)</f>
@@ -3090,55 +3121,55 @@
     <row r="23" spans="1:31">
       <c r="B23" s="2"/>
       <c r="D23" s="12">
-        <f t="shared" ref="D23:D33" si="28">D22+1</f>
+        <f t="shared" ref="D23:D33" si="36">D22+1</f>
         <v>1</v>
       </c>
       <c r="E23" s="5">
         <f>L6*(1-M6)*100</f>
-        <v>0.86897273598040858</v>
+        <v>1.2629668429383634</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="22"/>
-        <v>2.8743890100159772</v>
+        <f t="shared" si="30"/>
+        <v>1.4768739088587535</v>
       </c>
       <c r="G23" s="5">
-        <f t="shared" si="22"/>
-        <v>0.11211901101651393</v>
+        <f t="shared" si="30"/>
+        <v>4.1299605952425995E-2</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" si="22"/>
-        <v>5.16677470122184E-3</v>
+        <f t="shared" si="30"/>
+        <v>6.8275649146785156E-3</v>
       </c>
       <c r="I23" s="9">
-        <f t="shared" si="22"/>
-        <v>3.5632928973943721E-4</v>
+        <f t="shared" si="30"/>
+        <v>1.4323562758066816E-3</v>
       </c>
       <c r="K23" s="12">
-        <f t="shared" ref="K23:K33" si="29">K22+1</f>
+        <f t="shared" ref="K23:K33" si="37">K22+1</f>
         <v>1</v>
       </c>
       <c r="L23" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M23" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N23" s="16">
-        <f t="shared" si="25"/>
-        <v>15.136066487229382</v>
+        <f t="shared" si="33"/>
+        <v>5.5754468035775098</v>
       </c>
       <c r="O23" s="8">
-        <f t="shared" si="26"/>
-        <v>2.0925437539948453</v>
+        <f t="shared" si="34"/>
+        <v>2.7651637904447988</v>
       </c>
       <c r="P23" s="8">
-        <f t="shared" si="27"/>
-        <v>0.48104454114824025</v>
+        <f t="shared" si="35"/>
+        <v>1.9336809723390203</v>
       </c>
       <c r="S23" s="12">
-        <f t="shared" ref="S23:S33" si="30">S22+1</f>
+        <f t="shared" ref="S23:S33" si="38">S22+1</f>
         <v>1</v>
       </c>
       <c r="T23">
@@ -3158,7 +3189,7 @@
       </c>
       <c r="AA23">
         <f>SUMSQ(N22:P33)</f>
-        <v>468.96718245460033</v>
+        <v>83.809859704937026</v>
       </c>
       <c r="AC23" t="b">
         <f>$F$7=INT($F$7)</f>
@@ -3169,55 +3200,55 @@
       <c r="B24" s="2"/>
       <c r="C24" s="5"/>
       <c r="D24" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="E24" s="5">
         <f>L7*(1-M7)*100</f>
-        <v>3.7128835082799272</v>
+        <v>2.7057600906659642</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="22"/>
-        <v>3.0089979911152896E-2</v>
+        <f t="shared" si="30"/>
+        <v>3.4216440657571554E-2</v>
       </c>
       <c r="G24" s="5">
-        <f t="shared" si="22"/>
-        <v>0.11248904075584232</v>
+        <f t="shared" si="30"/>
+        <v>4.3932220103548664E-2</v>
       </c>
       <c r="H24" s="9">
-        <f t="shared" si="22"/>
-        <v>5.1838267629420428E-3</v>
+        <f t="shared" si="30"/>
+        <v>4.856668840926984E-3</v>
       </c>
       <c r="I24" s="9">
-        <f t="shared" si="22"/>
-        <v>3.5750529399600293E-4</v>
+        <f t="shared" si="30"/>
+        <v>6.3485867201659913E-4</v>
       </c>
       <c r="K24" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="L24" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M24" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N24" s="16">
-        <f t="shared" si="25"/>
-        <v>15.186020502038712</v>
+        <f t="shared" si="33"/>
+        <v>5.9308497139790699</v>
       </c>
       <c r="O24" s="8">
-        <f t="shared" si="26"/>
-        <v>2.0994498389915273</v>
+        <f t="shared" si="34"/>
+        <v>1.9669508805754286</v>
       </c>
       <c r="P24" s="8">
-        <f t="shared" si="27"/>
-        <v>0.48263214689460393</v>
+        <f t="shared" si="35"/>
+        <v>0.8570592072224088</v>
       </c>
       <c r="S24" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>2</v>
       </c>
       <c r="T24">
@@ -3248,56 +3279,56 @@
       <c r="B25" s="1"/>
       <c r="C25" s="5"/>
       <c r="D25" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>3</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" ref="E25:E30" si="31">L8*(1-M8)*100</f>
-        <v>2.1403390968608358</v>
+        <f t="shared" ref="E25:E30" si="39">L8*(1-M8)*100</f>
+        <v>34.240202074694871</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" ref="F25:I25" si="32">E25/(1-M8)*M8*(1-N8)</f>
-        <v>4.737608019846324E-2</v>
+        <f t="shared" ref="F25:I25" si="40">E25/(1-M8)*M8*(1-N8)</f>
+        <v>0.61508125467777441</v>
       </c>
       <c r="G25" s="5">
+        <f t="shared" si="40"/>
+        <v>1.086236211351478E-2</v>
+      </c>
+      <c r="H25" s="9">
+        <f t="shared" si="40"/>
+        <v>1.1615820757226788E-3</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="40"/>
+        <v>1.9621318846666872E-4</v>
+      </c>
+      <c r="K25" s="12">
+        <f t="shared" si="37"/>
+        <v>3</v>
+      </c>
+      <c r="L25" s="16">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="16">
         <f t="shared" si="32"/>
-        <v>7.6384710475654213E-5</v>
-      </c>
-      <c r="H25" s="9">
-        <f t="shared" si="32"/>
-        <v>8.5646037997174024E-5</v>
-      </c>
-      <c r="I25" s="9">
-        <f t="shared" si="32"/>
-        <v>2.4980094415842421E-5</v>
-      </c>
-      <c r="K25" s="12">
-        <f t="shared" si="29"/>
-        <v>3</v>
-      </c>
-      <c r="L25" s="16">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="16">
-        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N25" s="16">
-        <f t="shared" si="25"/>
-        <v>6.8746239428088794E-3</v>
+        <f t="shared" si="33"/>
+        <v>0.97761259021633018</v>
       </c>
       <c r="O25" s="8">
-        <f t="shared" si="26"/>
-        <v>1.9270358549364156E-2</v>
+        <f t="shared" si="34"/>
+        <v>0.26135596703760272</v>
       </c>
       <c r="P25" s="8">
-        <f t="shared" si="27"/>
-        <v>1.5737459481980725E-2</v>
+        <f t="shared" si="35"/>
+        <v>0.1236143087340013</v>
       </c>
       <c r="Q25" s="7"/>
       <c r="S25" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>3</v>
       </c>
       <c r="T25">
@@ -3317,7 +3348,7 @@
       </c>
       <c r="AA25" s="21">
         <f>AA23/AA24-(AA22/AA24)^2</f>
-        <v>12.052845750337932</v>
+        <v>1.9650585837513384</v>
       </c>
       <c r="AC25" t="b">
         <f>$F$9=INT($F$9)</f>
@@ -3327,56 +3358,56 @@
     <row r="26" spans="1:31">
       <c r="B26" s="5"/>
       <c r="D26" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>4</v>
       </c>
       <c r="E26" s="5">
+        <f t="shared" si="39"/>
+        <v>1.1717990377196337</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" ref="F26:I26" si="41">E26/(1-M9)*M9*(1-N9)</f>
+        <v>0.49206500374221962</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="41"/>
+        <v>8.4183306379739548E-3</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" si="41"/>
+        <v>1.1694306032613458E-3</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" si="41"/>
+        <v>1.8836466092800197E-4</v>
+      </c>
+      <c r="K26" s="12">
+        <f t="shared" si="37"/>
+        <v>4</v>
+      </c>
+      <c r="L26" s="16">
         <f t="shared" si="31"/>
-        <v>1.2705434700319609</v>
-      </c>
-      <c r="F26" s="5">
-        <f t="shared" ref="F26:I26" si="33">E26/(1-M9)*M9*(1-N9)</f>
-        <v>1.6393107335108386E-2</v>
-      </c>
-      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="M26" s="16">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="16">
         <f t="shared" si="33"/>
-        <v>5.4076595731083992E-5</v>
-      </c>
-      <c r="H26" s="9">
-        <f t="shared" si="33"/>
-        <v>5.9682216020714304E-6</v>
-      </c>
-      <c r="I26" s="9">
-        <f t="shared" si="33"/>
-        <v>4.6648168843776704E-6</v>
-      </c>
-      <c r="K26" s="12">
-        <f t="shared" si="29"/>
-        <v>4</v>
-      </c>
-      <c r="L26" s="16">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="16">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="16">
-        <f t="shared" si="25"/>
-        <v>3.8935148926380475E-3</v>
+        <v>0.60611980593412473</v>
       </c>
       <c r="O26" s="8">
-        <f t="shared" si="26"/>
-        <v>8.0570991627964314E-4</v>
+        <f t="shared" si="34"/>
+        <v>0.15787313144028167</v>
       </c>
       <c r="P26" s="8">
-        <f t="shared" si="27"/>
-        <v>1.6793340783759613E-3</v>
+        <f t="shared" si="35"/>
+        <v>6.7811277934080705E-2</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="S26" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="T26">
@@ -3403,56 +3434,56 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>5</v>
       </c>
       <c r="E27" s="5">
+        <f t="shared" si="39"/>
+        <v>1.6435296995853537</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" ref="F27:I27" si="42">E27/(1-M10)*M10*(1-N10)</f>
+        <v>2.2778373352040492E-2</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="42"/>
+        <v>6.3544818364061452E-3</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="42"/>
+        <v>8.4199003434816855E-4</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" si="42"/>
+        <v>1.3562255586816135E-4</v>
+      </c>
+      <c r="K27" s="12">
+        <f t="shared" si="37"/>
+        <v>5</v>
+      </c>
+      <c r="L27" s="16">
         <f t="shared" si="31"/>
-        <v>0.63938618925831192</v>
-      </c>
-      <c r="F27" s="5">
-        <f t="shared" ref="F27:I27" si="34">E27/(1-M10)*M10*(1-N10)</f>
-        <v>4.0874918947408408E-3</v>
-      </c>
-      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="M27" s="16">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="16">
+        <f t="shared" si="33"/>
+        <v>0.34314201916593184</v>
+      </c>
+      <c r="O27" s="8">
         <f t="shared" si="34"/>
-        <v>2.6329428633112058E-5</v>
-      </c>
-      <c r="H27" s="9">
-        <f t="shared" si="34"/>
-        <v>6.1250221696135376E-7</v>
-      </c>
-      <c r="I27" s="9">
-        <f t="shared" si="34"/>
-        <v>2.0416740565378455E-8</v>
-      </c>
-      <c r="K27" s="12">
-        <f t="shared" si="29"/>
-        <v>5</v>
-      </c>
-      <c r="L27" s="16">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M27" s="16">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="16">
-        <f t="shared" si="25"/>
-        <v>1.4217891461880512E-3</v>
-      </c>
-      <c r="O27" s="8">
-        <f t="shared" si="26"/>
-        <v>5.5125199526521836E-5</v>
+        <v>7.5779103091335176E-2</v>
       </c>
       <c r="P27" s="8">
-        <f t="shared" si="27"/>
-        <v>3.6750133017681219E-6</v>
+        <f t="shared" si="35"/>
+        <v>2.4412060056269044E-2</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="S27" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>5</v>
       </c>
       <c r="T27">
@@ -3478,56 +3509,56 @@
     <row r="28" spans="1:31">
       <c r="C28" s="5"/>
       <c r="D28" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>6</v>
       </c>
       <c r="E28" s="5">
+        <f t="shared" si="39"/>
+        <v>1.6435296995853537</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" ref="F28:I28" si="43">E28/(1-M11)*M11*(1-N11)</f>
+        <v>2.9523900224533169E-2</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="43"/>
+        <v>5.7027401095952588E-4</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="43"/>
+        <v>1.5822631517952161E-5</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="shared" si="43"/>
+        <v>4.709116523200048E-7</v>
+      </c>
+      <c r="K28" s="12">
+        <f t="shared" si="37"/>
+        <v>6</v>
+      </c>
+      <c r="L28" s="16">
         <f t="shared" si="31"/>
-        <v>0.51216726408542268</v>
-      </c>
-      <c r="F28" s="5">
-        <f t="shared" ref="F28:I28" si="35">E28/(1-M11)*M11*(1-N11)</f>
-        <v>2.6194459931257407E-3</v>
-      </c>
-      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="M28" s="16">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="16">
+        <f t="shared" si="33"/>
+        <v>1.5397398295907199E-2</v>
+      </c>
+      <c r="O28" s="8">
+        <f t="shared" si="34"/>
+        <v>7.1201841830784726E-4</v>
+      </c>
+      <c r="P28" s="8">
         <f t="shared" si="35"/>
-        <v>1.3545478361404114E-5</v>
-      </c>
-      <c r="H28" s="9">
-        <f t="shared" si="35"/>
-        <v>2.5255344745448636E-7</v>
-      </c>
-      <c r="I28" s="9">
-        <f t="shared" si="35"/>
-        <v>6.6901575484632147E-9</v>
-      </c>
-      <c r="K28" s="12">
-        <f t="shared" si="29"/>
-        <v>6</v>
-      </c>
-      <c r="L28" s="16">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M28" s="16">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="16">
-        <f t="shared" si="25"/>
-        <v>3.6572791575791106E-4</v>
-      </c>
-      <c r="O28" s="8">
-        <f t="shared" si="26"/>
-        <v>1.1364905135451887E-5</v>
-      </c>
-      <c r="P28" s="8">
-        <f t="shared" si="27"/>
-        <v>6.0211417936168932E-7</v>
+        <v>4.2382048708800429E-5</v>
       </c>
       <c r="Q28" s="7"/>
       <c r="S28" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>6</v>
       </c>
       <c r="T28">
@@ -3552,56 +3583,56 @@
     </row>
     <row r="29" spans="1:31">
       <c r="D29" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="E29" s="5">
+        <f t="shared" si="39"/>
+        <v>1.3737900924014981</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" ref="F29:I29" si="44">E29/(1-M12)*M12*(1-N12)</f>
+        <v>2.0570598252468614E-2</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="44"/>
+        <v>3.300196822682441E-4</v>
+      </c>
+      <c r="H29" s="9">
+        <f t="shared" si="44"/>
+        <v>9.1566154617778708E-6</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="shared" si="44"/>
+        <v>2.7251831731481757E-7</v>
+      </c>
+      <c r="K29" s="12">
+        <f t="shared" si="37"/>
+        <v>7</v>
+      </c>
+      <c r="L29" s="16">
         <f t="shared" si="31"/>
-        <v>0.38461918257314676</v>
-      </c>
-      <c r="F29" s="5">
-        <f t="shared" ref="F29:I29" si="36">E29/(1-M12)*M12*(1-N12)</f>
-        <v>1.475379660159755E-3</v>
-      </c>
-      <c r="G29" s="5">
-        <f t="shared" si="36"/>
-        <v>5.7418407826825143E-6</v>
-      </c>
-      <c r="H29" s="9">
-        <f t="shared" si="36"/>
-        <v>8.0438691149100656E-8</v>
-      </c>
-      <c r="I29" s="9">
-        <f t="shared" si="36"/>
-        <v>1.587605746363829E-9</v>
-      </c>
-      <c r="K29" s="12">
-        <f t="shared" si="29"/>
-        <v>7</v>
-      </c>
-      <c r="L29" s="16">
-        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M29" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N29" s="16">
-        <f t="shared" si="25"/>
-        <v>1.0335313408828526E-4</v>
+        <f t="shared" si="33"/>
+        <v>5.9403542808283936E-3</v>
       </c>
       <c r="O29" s="8">
-        <f t="shared" si="26"/>
-        <v>2.1718446610257178E-6</v>
+        <f t="shared" si="34"/>
+        <v>2.4722861746800251E-4</v>
       </c>
       <c r="P29" s="8">
-        <f t="shared" si="27"/>
-        <v>8.5730710303646762E-8</v>
+        <f t="shared" si="35"/>
+        <v>1.4715989135000149E-5</v>
       </c>
       <c r="Q29" s="7"/>
       <c r="S29" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="T29">
@@ -3626,55 +3657,55 @@
     </row>
     <row r="30" spans="1:31">
       <c r="D30" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>8</v>
       </c>
       <c r="E30" s="5">
+        <f t="shared" si="39"/>
+        <v>0.69212255796787792</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" ref="F30:I30" si="45">E30/(1-M13)*M13*(1-N13)</f>
+        <v>5.2020531059254367E-3</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="45"/>
+        <v>2.475147617011831E-5</v>
+      </c>
+      <c r="H30" s="9">
+        <f t="shared" si="45"/>
+        <v>6.8674615963334027E-7</v>
+      </c>
+      <c r="I30" s="9">
+        <f t="shared" si="45"/>
+        <v>2.0438873798611321E-8</v>
+      </c>
+      <c r="K30" s="12">
+        <f t="shared" si="37"/>
+        <v>8</v>
+      </c>
+      <c r="L30" s="16">
         <f t="shared" si="31"/>
-        <v>0.25674194472148432</v>
-      </c>
-      <c r="F30" s="5">
-        <f t="shared" ref="F30:I30" si="37">E30/(1-M13)*M13*(1-N13)</f>
-        <v>6.5658708852723582E-4</v>
-      </c>
-      <c r="G30" s="5">
-        <f t="shared" si="37"/>
-        <v>1.7093875204881984E-6</v>
-      </c>
-      <c r="H30" s="9">
-        <f t="shared" si="37"/>
-        <v>1.5993657889294869E-8</v>
-      </c>
-      <c r="I30" s="9">
-        <f t="shared" si="37"/>
-        <v>2.0906742338947541E-10</v>
-      </c>
-      <c r="K30" s="12">
-        <f t="shared" si="29"/>
-        <v>8</v>
-      </c>
-      <c r="L30" s="16">
-        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="M30" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N30" s="16">
-        <f t="shared" si="25"/>
-        <v>8.5469376024409917E-6</v>
+        <f t="shared" si="33"/>
+        <v>1.2375738085059154E-4</v>
       </c>
       <c r="O30" s="8">
-        <f t="shared" si="26"/>
-        <v>1.4394292100365382E-7</v>
+        <f t="shared" si="34"/>
+        <v>6.1807154367000622E-6</v>
       </c>
       <c r="P30" s="8">
-        <f t="shared" si="27"/>
-        <v>5.6448204315158362E-9</v>
+        <f t="shared" si="35"/>
+        <v>5.5184959256250564E-7</v>
       </c>
       <c r="S30" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="T30">
@@ -3699,55 +3730,55 @@
     </row>
     <row r="31" spans="1:31">
       <c r="D31" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>9</v>
       </c>
       <c r="E31" s="5">
         <f>L14*(1-M14)*100</f>
-        <v>0</v>
+        <v>0.27810362601126215</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" ref="F31:I33" si="38">E31/(1-M14)*M14*(1-N14)</f>
-        <v>0</v>
+        <f t="shared" ref="F31:I33" si="46">E31/(1-M14)*M14*(1-N14)</f>
+        <v>8.3368629221225931E-4</v>
       </c>
       <c r="G31" s="5">
+        <f t="shared" si="46"/>
+        <v>2.6854173002855986E-6</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="46"/>
+        <v>2.9824404646933648E-8</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="shared" si="46"/>
+        <v>3.488234461629666E-10</v>
+      </c>
+      <c r="K31" s="12">
+        <f t="shared" si="37"/>
+        <v>9</v>
+      </c>
+      <c r="L31" s="16">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="16">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="16">
+        <f t="shared" si="33"/>
+        <v>1.3427086501427993E-5</v>
+      </c>
+      <c r="O31" s="8">
+        <f t="shared" si="34"/>
+        <v>2.6841964182240286E-7</v>
+      </c>
+      <c r="P31" s="8">
+        <f t="shared" si="35"/>
+        <v>6.2788220309333991E-9</v>
+      </c>
+      <c r="S31" s="12">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="9">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="9">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="K31" s="12">
-        <f t="shared" si="29"/>
-        <v>9</v>
-      </c>
-      <c r="L31" s="16">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M31" s="16">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="16">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="8">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="8">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="S31" s="12">
-        <f t="shared" si="30"/>
         <v>9</v>
       </c>
       <c r="T31">
@@ -3772,55 +3803,55 @@
     </row>
     <row r="32" spans="1:31">
       <c r="D32" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>10</v>
       </c>
       <c r="E32" s="5">
         <f>L15*(1-M15)*100</f>
-        <v>0.38461918257314676</v>
+        <v>0.69212255796787792</v>
       </c>
       <c r="F32" s="5">
+        <f t="shared" si="46"/>
+        <v>5.1850806651230702E-3</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" si="46"/>
+        <v>4.1488188628007826E-5</v>
+      </c>
+      <c r="H32" s="9">
+        <f t="shared" si="46"/>
+        <v>9.2656227887037973E-7</v>
+      </c>
+      <c r="I32" s="9">
+        <f t="shared" si="46"/>
+        <v>1.6351099038889053E-8</v>
+      </c>
+      <c r="K32" s="12">
+        <f t="shared" si="37"/>
+        <v>10</v>
+      </c>
+      <c r="L32" s="16">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="16">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="16">
+        <f t="shared" si="33"/>
+        <v>1.2446456588402347E-4</v>
+      </c>
+      <c r="O32" s="8">
+        <f t="shared" si="34"/>
+        <v>6.4859359520926578E-6</v>
+      </c>
+      <c r="P32" s="8">
+        <f t="shared" si="35"/>
+        <v>2.9431978270000296E-7</v>
+      </c>
+      <c r="S32" s="12">
         <f t="shared" si="38"/>
-        <v>1.475379660159755E-3</v>
-      </c>
-      <c r="G32" s="5">
-        <f t="shared" si="38"/>
-        <v>5.7144986837173595E-6</v>
-      </c>
-      <c r="H32" s="9">
-        <f t="shared" si="38"/>
-        <v>1.0654598564486141E-7</v>
-      </c>
-      <c r="I32" s="9">
-        <f t="shared" si="38"/>
-        <v>2.8224102157579181E-9</v>
-      </c>
-      <c r="K32" s="12">
-        <f t="shared" si="29"/>
-        <v>10</v>
-      </c>
-      <c r="L32" s="16">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="16">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="16">
-        <f t="shared" si="25"/>
-        <v>1.7143496051152078E-5</v>
-      </c>
-      <c r="O32" s="8">
-        <f t="shared" si="26"/>
-        <v>7.4582189951402983E-7</v>
-      </c>
-      <c r="P32" s="8">
-        <f t="shared" si="27"/>
-        <v>5.0803383883642527E-8</v>
-      </c>
-      <c r="S32" s="12">
-        <f t="shared" si="30"/>
         <v>10</v>
       </c>
       <c r="T32">
@@ -3845,55 +3876,55 @@
     </row>
     <row r="33" spans="2:29">
       <c r="D33" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="36"/>
         <v>11</v>
       </c>
       <c r="E33" s="5">
         <f>L16*(1-M16)*100</f>
-        <v>1.6474274786295244</v>
+        <v>0.55453444825704301</v>
       </c>
       <c r="F33" s="5">
+        <f t="shared" si="46"/>
+        <v>3.3130204446220079E-3</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="46"/>
+        <v>3.0776692654958541E-5</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="46"/>
+        <v>1.7057466517369066E-6</v>
+      </c>
+      <c r="I33" s="9">
+        <f t="shared" si="46"/>
+        <v>1.0464703384888997E-7</v>
+      </c>
+      <c r="K33" s="12">
+        <f t="shared" si="37"/>
+        <v>11</v>
+      </c>
+      <c r="L33" s="16">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="16">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="16">
+        <f t="shared" si="33"/>
+        <v>9.2330077964875623E-5</v>
+      </c>
+      <c r="O33" s="8">
+        <f t="shared" si="34"/>
+        <v>1.1940226562158346E-5</v>
+      </c>
+      <c r="P33" s="8">
+        <f t="shared" si="35"/>
+        <v>9.418233046400097E-7</v>
+      </c>
+      <c r="S33" s="12">
         <f t="shared" si="38"/>
-        <v>2.5270406354631032E-2</v>
-      </c>
-      <c r="G33" s="5">
-        <f t="shared" si="38"/>
-        <v>3.8672664776314992E-4</v>
-      </c>
-      <c r="H33" s="9">
-        <f t="shared" si="38"/>
-        <v>1.6070803768525584E-5</v>
-      </c>
-      <c r="I33" s="9">
-        <f t="shared" si="38"/>
-        <v>9.906659857310291E-7</v>
-      </c>
-      <c r="K33" s="12">
-        <f t="shared" si="29"/>
-        <v>11</v>
-      </c>
-      <c r="L33" s="16">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M33" s="16">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="16">
-        <f t="shared" si="25"/>
-        <v>1.1601799432894497E-3</v>
-      </c>
-      <c r="O33" s="8">
-        <f t="shared" si="26"/>
-        <v>1.1249562637967908E-4</v>
-      </c>
-      <c r="P33" s="8">
-        <f t="shared" si="27"/>
-        <v>8.9159938715792623E-6</v>
-      </c>
-      <c r="S33" s="12">
-        <f t="shared" si="30"/>
         <v>11</v>
       </c>
       <c r="T33">
@@ -4787,23 +4818,23 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <f t="shared" ref="E59:I59" si="39">E15-TRUNC(E15)</f>
+        <f t="shared" ref="E59:I59" si="47">E15-TRUNC(E15)</f>
         <v>0</v>
       </c>
       <c r="F59">
-        <f t="shared" si="39"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="G59">
-        <f t="shared" si="39"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="H59">
-        <f t="shared" si="39"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="I59">
-        <f t="shared" si="39"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AC59" t="b">
@@ -4822,8 +4853,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AQ59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5:X16"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelCol="1"/>
@@ -4854,30 +4885,30 @@
       </c>
       <c r="AC1">
         <f>MIN($AA$14)</f>
-        <v>86.087894641279703</v>
+        <v>7.8361878140470598</v>
       </c>
       <c r="AG1">
         <v>1</v>
       </c>
       <c r="AH1" s="6">
         <f t="shared" ref="AH1:AL1" si="0">3*L5</f>
-        <v>1.4563106796116505</v>
+        <v>0.67264573991031396</v>
       </c>
       <c r="AI1" s="6">
         <f t="shared" si="0"/>
-        <v>1.0150375939849623</v>
+        <v>0.15151515151515152</v>
       </c>
       <c r="AJ1" s="6">
         <f t="shared" si="0"/>
-        <v>1.1020408163265307</v>
+        <v>0.1744186046511628</v>
       </c>
       <c r="AK1" s="6">
         <f t="shared" si="0"/>
-        <v>7.3170731707317083E-2</v>
+        <v>0.5325443786982248</v>
       </c>
       <c r="AL1" s="6">
         <f t="shared" si="0"/>
-        <v>0.10204081632653061</v>
+        <v>0.36809815950920244</v>
       </c>
       <c r="AM1">
         <v>1</v>
@@ -4915,7 +4946,7 @@
       </c>
       <c r="AC3" t="b">
         <f>$AA$11&gt;=0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3" s="12" t="s">
         <v>61</v>
@@ -5002,30 +5033,30 @@
       </c>
       <c r="AF4" s="22">
         <f>PRODUCT(AH4:AL4)</f>
-        <v>-5.8273251136394943E-4</v>
+        <v>6.773482186402971E-2</v>
       </c>
       <c r="AG4" s="5">
         <v>1</v>
       </c>
       <c r="AH4" s="6">
         <f>1-AH1</f>
-        <v>-0.4563106796116505</v>
+        <v>0.32735426008968604</v>
       </c>
       <c r="AI4" s="6">
         <f t="shared" ref="AI4:AL4" si="1">1-AI1</f>
-        <v>-1.5037593984962294E-2</v>
+        <v>0.84848484848484851</v>
       </c>
       <c r="AJ4" s="6">
         <f t="shared" si="1"/>
-        <v>-0.10204081632653073</v>
+        <v>0.82558139534883723</v>
       </c>
       <c r="AK4" s="6">
         <f t="shared" si="1"/>
-        <v>0.92682926829268286</v>
+        <v>0.4674556213017752</v>
       </c>
       <c r="AL4" s="6">
         <f t="shared" si="1"/>
-        <v>0.89795918367346939</v>
+        <v>0.63190184049079756</v>
       </c>
       <c r="AM4" s="5">
         <v>1</v>
@@ -5046,42 +5077,42 @@
       </c>
       <c r="F5">
         <f>Base!F5</f>
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="G5">
         <f>Base!G5</f>
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="H5">
         <f>Base!H5</f>
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="I5">
         <f>Base!I5</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="K5" s="12">
         <v>0</v>
       </c>
       <c r="L5" s="6">
         <f t="shared" ref="L5:P16" si="2">E5/E$17</f>
-        <v>0.4854368932038835</v>
+        <v>0.22421524663677131</v>
       </c>
       <c r="M5" s="6">
         <f t="shared" si="2"/>
-        <v>0.33834586466165412</v>
+        <v>5.0505050505050504E-2</v>
       </c>
       <c r="N5" s="6">
         <f t="shared" si="2"/>
-        <v>0.36734693877551022</v>
+        <v>5.8139534883720929E-2</v>
       </c>
       <c r="O5" s="6">
         <f t="shared" si="2"/>
-        <v>2.4390243902439025E-2</v>
+        <v>0.17751479289940827</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="2"/>
-        <v>3.4013605442176874E-2</v>
+        <v>0.12269938650306748</v>
       </c>
       <c r="Q5" s="7">
         <v>0</v>
@@ -5092,19 +5123,19 @@
       </c>
       <c r="U5" t="str">
         <f t="shared" si="3"/>
-        <v>x90 0</v>
+        <v>x20 0</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" si="3"/>
-        <v>x90 0</v>
+        <v>x20 0</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="3"/>
-        <v>x5 0</v>
+        <v>x30 0</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" si="3"/>
-        <v>x5 0</v>
+        <v>x20 0</v>
       </c>
       <c r="Z5" s="12" t="s">
         <v>48</v>
@@ -5121,28 +5152,28 @@
       </c>
       <c r="AF5" s="22">
         <f>SUM(AH5:AL5)</f>
-        <v>4.7375515448703873E-2</v>
+        <v>0.28221024889539736</v>
       </c>
       <c r="AG5" s="5"/>
       <c r="AH5" s="6">
         <f>PRODUCT($AG4:AG4,AI4:$AM4)*AH1</f>
-        <v>1.859784610736009E-3</v>
+        <v>0.13918114081649946</v>
       </c>
       <c r="AI5" s="6">
         <f>PRODUCT($AG4:AH4,AJ4:$AM4)*AI1</f>
-        <v>3.9334444517066879E-2</v>
+        <v>1.2095503904291023E-2</v>
       </c>
       <c r="AJ5" s="6">
         <f>PRODUCT($AG4:AI4,AK4:$AM4)*AJ1</f>
-        <v>6.2935111227306485E-3</v>
+        <v>1.4310173633245713E-2</v>
       </c>
       <c r="AK5" s="6">
         <f>PRODUCT($AG4:AJ4,AL4:$AM4)*AK1</f>
-        <v>-4.6005198265574969E-5</v>
+        <v>7.7166252756489528E-2</v>
       </c>
       <c r="AL5" s="6">
         <f>PRODUCT($AG4:AK4,AM4:$AM4)*AL1</f>
-        <v>-6.6219603564085169E-5</v>
+        <v>3.9457177784871678E-2</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -5158,22 +5189,22 @@
       </c>
       <c r="E6">
         <f>Base!E6</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>100</v>
       </c>
       <c r="G6">
         <f>Base!G6</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H6">
         <f>Base!H6</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="I6">
         <f>Base!I6</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="K6" s="12">
         <f t="shared" ref="K6:K16" si="5">K5+1</f>
@@ -5181,30 +5212,30 @@
       </c>
       <c r="L6" s="6">
         <f t="shared" si="2"/>
-        <v>0.14563106796116504</v>
+        <v>4.4843049327354258E-2</v>
       </c>
       <c r="M6" s="6">
         <f t="shared" si="2"/>
-        <v>0.37593984962406013</v>
+        <v>0.25252525252525254</v>
       </c>
       <c r="N6" s="6">
         <f t="shared" si="2"/>
-        <v>0.12244897959183673</v>
+        <v>5.8139534883720929E-2</v>
       </c>
       <c r="O6" s="6">
         <f t="shared" si="2"/>
-        <v>4.878048780487805E-2</v>
+        <v>0.17751479289940827</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="2"/>
-        <v>6.8027210884353748E-2</v>
+        <v>0.18404907975460122</v>
       </c>
       <c r="Q6" s="7">
         <v>0</v>
       </c>
       <c r="T6" t="str">
         <f t="shared" si="3"/>
-        <v>x30 1</v>
+        <v>x20 1</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" si="3"/>
@@ -5212,77 +5243,77 @@
       </c>
       <c r="V6" t="str">
         <f t="shared" si="3"/>
-        <v>x30 1</v>
+        <v>x20 1</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="3"/>
-        <v>x10 1</v>
+        <v>x30 1</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" si="3"/>
-        <v>x10 1</v>
+        <v>x30 1</v>
       </c>
       <c r="Z6" s="12" t="s">
         <v>50</v>
       </c>
       <c r="AA6" s="5">
         <f>B9-(AA4-AA5)</f>
-        <v>174.66445843642995</v>
+        <v>9.0517548906732515</v>
       </c>
       <c r="AB6" s="19" t="s">
         <v>37</v>
       </c>
       <c r="AC6" t="b">
         <f>$AA$7&gt;=0</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <v>2</v>
       </c>
       <c r="AF6" s="23">
         <f>SUM(AH6:AQ6)</f>
-        <v>-0.56129299742397065</v>
+        <v>0.38686639643407339</v>
       </c>
       <c r="AG6" s="5"/>
       <c r="AH6" s="6">
         <f>PRODUCT(AH4:AJ4)*PRODUCT(AK1,AL1)</f>
-        <v>-5.2278634392698829E-6</v>
+        <v>4.4951215197955058E-2</v>
       </c>
       <c r="AI6" s="6">
         <f>PRODUCT(AH4:AI4,AK4)*PRODUCT(AJ1,AL1)</f>
-        <v>7.1517171849211922E-4</v>
+        <v>8.3360234756771137E-3</v>
       </c>
       <c r="AJ6" s="6">
         <f>PRODUCT(AH4:AI4,AL4)*PRODUCT(AJ1,AK1)</f>
-        <v>4.968561412682091E-4</v>
+        <v>1.6302729455596375E-2</v>
       </c>
       <c r="AK6" s="6">
         <f>PRODUCT(AH4,AJ4,AK4)*PRODUCT(AI1,AL1)</f>
-        <v>4.4698232405757828E-3</v>
+        <v>7.0459246044413714E-3</v>
       </c>
       <c r="AL6" s="6">
         <f>PRODUCT(AH4,AJ4,AL4)*PRODUCT(AI1,AK1)</f>
-        <v>3.105350882926333E-3</v>
+        <v>1.3779687992230274E-2</v>
       </c>
       <c r="AM6" s="6">
         <f>PRODUCT(AH4,AK4,AL4)*PRODUCT(AI1,AJ1)</f>
-        <v>-0.42481200078432185</v>
+        <v>2.5553881487938774E-3</v>
       </c>
       <c r="AN6" s="6">
         <f>PRODUCT(AI4,AJ4,AK4)*PRODUCT(AH1,AL1)</f>
-        <v>2.1133916031091009E-4</v>
+        <v>8.1076392708640449E-2</v>
       </c>
       <c r="AO6" s="6">
         <f>PRODUCT(AI4,AJ4,AL4)*PRODUCT(AH1,AK1)</f>
-        <v>1.4682510084757969E-4</v>
+        <v>0.1585607933352525</v>
       </c>
       <c r="AP6" s="6">
         <f>PRODUCT(AI4,AK4,AL4)*PRODUCT(AH1,AJ1)</f>
-        <v>-2.0085673795948878E-2</v>
+        <v>2.9404466369682979E-2</v>
       </c>
       <c r="AQ6" s="6">
         <f>PRODUCT(AJ4,AK4,AL4)*PRODUCT(AH1,AI1)</f>
-        <v>-0.12553546122468154</v>
+        <v>2.4853775145803472E-2</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -5299,22 +5330,22 @@
       </c>
       <c r="E7">
         <f>Base!E7</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <f>Base!F7</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G7">
         <v>100</v>
       </c>
       <c r="H7">
         <f>Base!H7</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I7">
         <f>Base!I7</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" si="5"/>
@@ -5322,34 +5353,34 @@
       </c>
       <c r="L7" s="6">
         <f t="shared" si="2"/>
-        <v>0.14563106796116504</v>
+        <v>4.4843049327354258E-2</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" si="2"/>
-        <v>0.11278195488721804</v>
+        <v>5.0505050505050504E-2</v>
       </c>
       <c r="N7" s="6">
         <f t="shared" si="2"/>
-        <v>0.40816326530612246</v>
+        <v>0.29069767441860467</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" si="2"/>
-        <v>4.878048780487805E-2</v>
+        <v>0.11834319526627218</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="2"/>
-        <v>6.8027210884353748E-2</v>
+        <v>0.12269938650306748</v>
       </c>
       <c r="Q7" s="7">
         <v>0</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="3"/>
-        <v>x30 2</v>
+        <v>x20 2</v>
       </c>
       <c r="U7" t="str">
         <f t="shared" si="3"/>
-        <v>x30 2</v>
+        <v>x20 2</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="3"/>
@@ -5357,18 +5388,18 @@
       </c>
       <c r="W7" t="str">
         <f t="shared" si="3"/>
-        <v>x10 2</v>
+        <v>x20 2</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="3"/>
-        <v>x10 2</v>
+        <v>x20 2</v>
       </c>
       <c r="Z7" s="12" t="s">
         <v>51</v>
       </c>
       <c r="AA7" s="5">
         <f>(AA4+AA5)-B9</f>
-        <v>-134.66445843642995</v>
+        <v>30.948245109326749</v>
       </c>
       <c r="AB7" s="19" t="s">
         <v>37</v>
@@ -5382,48 +5413,48 @@
       </c>
       <c r="AF7" s="23">
         <f>SUM(AH7:AQ7)</f>
-        <v>1.2463528654218718</v>
+        <v>0.21295975304203327</v>
       </c>
       <c r="AG7" s="5"/>
       <c r="AH7" s="6">
         <f>PRODUCT(AH1:AJ1)*PRODUCT(AK4,AL4)</f>
-        <v>1.3557829812265592</v>
+        <v>5.250797566014819E-3</v>
       </c>
       <c r="AI7" s="6">
         <f>PRODUCT(AH1:AI1,AK1)*PRODUCT(AJ4,AL4)</f>
-        <v>-9.9106943072117017E-3</v>
+        <v>2.8314427381295085E-2</v>
       </c>
       <c r="AJ7" s="6">
         <f>PRODUCT(AH1:AI1,AL1)*PRODUCT(AJ4,AK4)</f>
-        <v>-1.4265393320986537E-2</v>
+        <v>1.4477927269400078E-2</v>
       </c>
       <c r="AK7" s="6">
         <f>PRODUCT(AH1,AJ1,AK1)*PRODUCT(AI4,AL4)</f>
-        <v>-1.5857110891538591E-3</v>
+        <v>3.3498759155335033E-2</v>
       </c>
       <c r="AL7" s="6">
         <f>PRODUCT(AH1,AJ1,AL1)*PRODUCT(AI4,AK4)</f>
-        <v>-2.2824629313578271E-3</v>
+        <v>1.7128815360980376E-2</v>
       </c>
       <c r="AM7" s="6">
         <f>PRODUCT(AH1,AK1,AL1)*PRODUCT(AI4,AJ4)</f>
-        <v>1.6684670550861329E-5</v>
+        <v>9.2365510680729596E-2</v>
       </c>
       <c r="AN7" s="6">
         <f>PRODUCT(AI1,AJ1,AK1)*PRODUCT(AH4,AL4)</f>
-        <v>-3.3537789535604358E-2</v>
+        <v>2.9112016884993539E-3</v>
       </c>
       <c r="AO7" s="6">
         <f>PRODUCT(AI1,AJ1,AL1)*PRODUCT(AH4,AK4)</f>
-        <v>-4.8274090998218389E-2</v>
+        <v>1.4885756206566274E-3</v>
       </c>
       <c r="AP7" s="6">
         <f>PRODUCT(AI1,AK1,AL1)*PRODUCT(AH4,AJ4)</f>
-        <v>3.528807821507197E-4</v>
+        <v>8.0270027139205478E-3</v>
       </c>
       <c r="AQ7" s="6">
         <f>PRODUCT(AJ1,AK1,AL1)*PRODUCT(AH4,AI4)</f>
-        <v>5.6460925144114675E-5</v>
+        <v>9.4967356052017733E-3</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -5439,23 +5470,23 @@
       </c>
       <c r="E8">
         <f>Base!E8</f>
-        <v>17</v>
+        <v>250</v>
       </c>
       <c r="F8">
         <f>Base!F8</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <f>Base!G8</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H8">
         <f>Base!H8</f>
-        <v>126</v>
+        <v>20</v>
       </c>
       <c r="I8">
         <f>Base!I8</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K8" s="12">
         <f t="shared" si="5"/>
@@ -5463,46 +5494,46 @@
       </c>
       <c r="L8" s="6">
         <f t="shared" si="2"/>
-        <v>8.2524271844660199E-2</v>
+        <v>0.5605381165919282</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="2"/>
-        <v>6.3909774436090222E-2</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="2"/>
-        <v>1.2244897959183673E-2</v>
+        <v>3.4883720930232558E-2</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="2"/>
-        <v>0.61463414634146341</v>
+        <v>0.11834319526627218</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="2"/>
-        <v>0.23809523809523808</v>
+        <v>0.15337423312883436</v>
       </c>
       <c r="Q8" s="7">
         <v>0</v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="3"/>
-        <v>x17 3</v>
+        <v>x250 3</v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="3"/>
-        <v>x17 3</v>
+        <v>x12 3</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="3"/>
-        <v>x3 3</v>
+        <v>x12 3</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="3"/>
-        <v>x126 3</v>
+        <v>x20 3</v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="3"/>
-        <v>x35 3</v>
+        <v>x25 3</v>
       </c>
       <c r="AC8" t="b">
         <f>$AA$16&gt;=$AA$17</f>
@@ -5513,27 +5544,27 @@
       </c>
       <c r="AF8" s="23">
         <f>SUM(AH8:AL8)</f>
-        <v>0.25598422423318046</v>
+        <v>4.6744165427919537E-2</v>
       </c>
       <c r="AH8" s="24">
         <f>PRODUCT($AG1:AG1,AI1:$AM1)*AH4</f>
-        <v>-3.8111124472277685E-3</v>
+        <v>1.6958456437860311E-3</v>
       </c>
       <c r="AI8" s="24">
         <f>PRODUCT($AG1:AH1,AJ1:$AM1)*AI4</f>
-        <v>-1.8019444194930216E-4</v>
+        <v>1.9513840284661185E-2</v>
       </c>
       <c r="AJ8" s="24">
         <f>PRODUCT($AG1:AI1,AK1:$AM1)*AJ4</f>
-        <v>-1.1262152621831479E-3</v>
+        <v>1.649384119298743E-2</v>
       </c>
       <c r="AK8" s="24">
         <f>PRODUCT($AG1:AJ1,AL1:$AM1)*AK4</f>
-        <v>0.15406624786665443</v>
+        <v>3.0587170287464959E-3</v>
       </c>
       <c r="AL8" s="24">
         <f>PRODUCT($AG1:AK1,AM1:$AM1)*AL4</f>
-        <v>0.10703549851788627</v>
+        <v>5.9819212777383994E-3</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -5542,7 +5573,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM(L22:P33)</f>
-        <v>204.66445843642995</v>
+        <v>39.051754890673251</v>
       </c>
       <c r="D9" s="12">
         <f t="shared" si="4"/>
@@ -5550,23 +5581,23 @@
       </c>
       <c r="E9">
         <f>Base!E9</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <f>Base!F9</f>
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="G9">
         <f>Base!G9</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H9">
         <f>Base!H9</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I9">
         <f>Base!I9</f>
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="K9" s="12">
         <f t="shared" si="5"/>
@@ -5574,46 +5605,46 @@
       </c>
       <c r="L9" s="6">
         <f t="shared" si="2"/>
-        <v>4.8543689320388349E-2</v>
+        <v>2.6905829596412557E-2</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="2"/>
-        <v>3.7593984962406013E-2</v>
+        <v>0.50505050505050508</v>
       </c>
       <c r="N9" s="6">
         <f t="shared" si="2"/>
-        <v>1.2244897959183673E-2</v>
+        <v>3.4883720930232558E-2</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="2"/>
-        <v>0.17073170731707318</v>
+        <v>0.14792899408284024</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>0.46258503401360546</v>
+        <v>0.14723926380368099</v>
       </c>
       <c r="Q9" s="7">
         <v>0</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="3"/>
-        <v>x10 4</v>
+        <v>x12 4</v>
       </c>
       <c r="U9" t="str">
         <f t="shared" si="3"/>
-        <v>x10 4</v>
+        <v>x200 4</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="3"/>
-        <v>x3 4</v>
+        <v>x12 4</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="3"/>
-        <v>x35 4</v>
+        <v>x25 4</v>
       </c>
       <c r="X9" t="str">
         <f t="shared" si="3"/>
-        <v>x68 4</v>
+        <v>x24 4</v>
       </c>
       <c r="Z9" s="12" t="s">
         <v>52</v>
@@ -5630,7 +5661,7 @@
       </c>
       <c r="AF9" s="23">
         <f>PRODUCT(AH1:AL1)</f>
-        <v>1.2163124831577984E-2</v>
+        <v>3.48461433654664E-3</v>
       </c>
       <c r="AG9" s="5"/>
     </row>
@@ -5640,7 +5671,7 @@
       </c>
       <c r="B10" s="5">
         <f>100*(1-(1-SUMIF(T22:X33,"&lt;&gt;0",E22:I33)/100)^B6)</f>
-        <v>12.727049881970276</v>
+        <v>2.7523261435854041</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -5651,23 +5682,23 @@
       </c>
       <c r="E10">
         <f>Base!E10</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <f>Base!F10</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <f>Base!G10</f>
-        <v>5</v>
+        <v>150</v>
       </c>
       <c r="H10">
         <f>Base!H10</f>
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="I10">
         <f>Base!I10</f>
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="5"/>
@@ -5675,46 +5706,46 @@
       </c>
       <c r="L10" s="6">
         <f t="shared" si="2"/>
-        <v>2.4271844660194174E-2</v>
+        <v>2.6905829596412557E-2</v>
       </c>
       <c r="M10" s="6">
         <f t="shared" si="2"/>
-        <v>1.8796992481203006E-2</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="N10" s="6">
         <f t="shared" si="2"/>
-        <v>2.0408163265306121E-2</v>
+        <v>0.43604651162790697</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="2"/>
-        <v>2.4390243902439025E-2</v>
+        <v>0.14201183431952663</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
-        <v>3.4013605442176874E-2</v>
+        <v>0.14723926380368099</v>
       </c>
       <c r="Q10" s="7">
         <v>0</v>
       </c>
       <c r="T10" t="str">
         <f t="shared" si="3"/>
-        <v>x5 5</v>
+        <v>x12 5</v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="3"/>
-        <v>x5 5</v>
+        <v>x12 5</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="3"/>
-        <v>x5 5</v>
+        <v>x150 5</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="3"/>
-        <v>x5 5</v>
+        <v>x24 5</v>
       </c>
       <c r="X10" t="str">
         <f t="shared" si="3"/>
-        <v>x5 5</v>
+        <v>x24 5</v>
       </c>
       <c r="Z10" s="12" t="s">
         <v>53</v>
@@ -5728,7 +5759,7 @@
       </c>
       <c r="AF10" s="22">
         <f>SUM(AF4:AF9)</f>
-        <v>0.99999999999999956</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -5737,7 +5768,7 @@
       </c>
       <c r="B11" s="5">
         <f>1/$B$6*(1/100*SUMPRODUCT(F22:I33,U22:X33,U22:X33)-(1/100*SUMPRODUCT(F22:I33,U22:X33))^2)</f>
-        <v>41.519568377514553</v>
+        <v>12.130760183996218</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -5748,23 +5779,23 @@
       </c>
       <c r="E11">
         <f>Base!E11</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <f>Base!F11</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G11">
         <f>Base!G11</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H11">
         <f>Base!H11</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11">
         <f>Base!I11</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="5"/>
@@ -5772,53 +5803,53 @@
       </c>
       <c r="L11" s="6">
         <f t="shared" si="2"/>
-        <v>1.9417475728155338E-2</v>
+        <v>2.6905829596412557E-2</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" si="2"/>
-        <v>1.5037593984962405E-2</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="N11" s="6">
         <f t="shared" si="2"/>
-        <v>1.6326530612244899E-2</v>
+        <v>3.4883720930232558E-2</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="2"/>
-        <v>1.9512195121951219E-2</v>
+        <v>2.9585798816568046E-2</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>2.7210884353741496E-2</v>
+        <v>3.0674846625766871E-2</v>
       </c>
       <c r="Q11" s="7">
         <v>0</v>
       </c>
       <c r="T11" t="str">
         <f t="shared" si="3"/>
-        <v>x4 6</v>
+        <v>x12 6</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" si="3"/>
-        <v>x4 6</v>
+        <v>x12 6</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="3"/>
-        <v>x4 6</v>
+        <v>x12 6</v>
       </c>
       <c r="W11" t="str">
         <f t="shared" si="3"/>
-        <v>x4 6</v>
+        <v>x5 6</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="3"/>
-        <v>x4 6</v>
+        <v>x5 6</v>
       </c>
       <c r="Z11" s="12" t="s">
         <v>54</v>
       </c>
       <c r="AA11" s="5">
         <f>B10-(AA9-AA10)</f>
-        <v>2.7270498819702755</v>
+        <v>-7.2476738564145959</v>
       </c>
       <c r="AB11" s="19" t="s">
         <v>37</v>
@@ -5834,7 +5865,7 @@
       </c>
       <c r="B12" s="5">
         <f>SQRT(B11)</f>
-        <v>6.4435679850153322</v>
+        <v>3.4829240853047914</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -5845,23 +5876,23 @@
       </c>
       <c r="E12">
         <f>Base!E12</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <f>Base!F12</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <f>Base!G12</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <f>Base!H12</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <f>Base!I12</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K12" s="12">
         <f t="shared" si="5"/>
@@ -5869,53 +5900,53 @@
       </c>
       <c r="L12" s="6">
         <f t="shared" si="2"/>
-        <v>1.4563106796116505E-2</v>
+        <v>2.2421524663677129E-2</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="2"/>
-        <v>1.1278195488721804E-2</v>
+        <v>2.5252525252525252E-2</v>
       </c>
       <c r="N12" s="6">
         <f t="shared" si="2"/>
-        <v>1.2244897959183673E-2</v>
+        <v>2.9069767441860465E-2</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="2"/>
-        <v>1.4634146341463415E-2</v>
+        <v>2.9585798816568046E-2</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="2"/>
-        <v>2.0408163265306121E-2</v>
+        <v>3.0674846625766871E-2</v>
       </c>
       <c r="Q12" s="7">
         <v>0</v>
       </c>
       <c r="T12" t="str">
         <f t="shared" si="3"/>
-        <v>x3 7</v>
+        <v>x10 7</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="3"/>
-        <v>x3 7</v>
+        <v>x10 7</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="3"/>
-        <v>x3 7</v>
+        <v>x10 7</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="3"/>
-        <v>x3 7</v>
+        <v>x5 7</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="3"/>
-        <v>x3 7</v>
+        <v>x5 7</v>
       </c>
       <c r="Z12" s="12" t="s">
         <v>55</v>
       </c>
       <c r="AA12" s="5">
         <f>(AA9+AA10)-B10</f>
-        <v>27.272950118029726</v>
+        <v>37.247673856414593</v>
       </c>
       <c r="AB12" s="19" t="s">
         <v>37</v>
@@ -5929,11 +5960,11 @@
       </c>
       <c r="AF12" s="23">
         <f>SUM(AF13:AF15)</f>
-        <v>1.5145002144866302</v>
+        <v>0.2631885328064994</v>
       </c>
       <c r="AG12">
         <f>1/AF12</f>
-        <v>0.66028382857573231</v>
+        <v>3.7995576377760223</v>
       </c>
     </row>
     <row r="13" spans="1:43">
@@ -5946,23 +5977,23 @@
       </c>
       <c r="E13">
         <f>Base!E13</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F13">
         <f>Base!F13</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G13">
         <f>Base!G13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13">
         <f>Base!H13</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I13">
         <f>Base!I13</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K13" s="12">
         <f t="shared" si="5"/>
@@ -5970,46 +6001,46 @@
       </c>
       <c r="L13" s="6">
         <f t="shared" si="2"/>
-        <v>9.7087378640776691E-3</v>
+        <v>1.1210762331838564E-2</v>
       </c>
       <c r="M13" s="6">
         <f t="shared" si="2"/>
-        <v>7.5187969924812026E-3</v>
+        <v>1.2626262626262626E-2</v>
       </c>
       <c r="N13" s="6">
         <f t="shared" si="2"/>
-        <v>8.1632653061224497E-3</v>
+        <v>8.7209302325581394E-3</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" si="2"/>
-        <v>9.7560975609756097E-3</v>
+        <v>2.9585798816568046E-2</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" si="2"/>
-        <v>1.3605442176870748E-2</v>
+        <v>3.0674846625766871E-2</v>
       </c>
       <c r="Q13" s="7">
         <v>0</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="3"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="3"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="3"/>
-        <v>x2 8</v>
+        <v>x3 8</v>
       </c>
       <c r="W13" t="str">
         <f t="shared" si="3"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="3"/>
-        <v>x2 8</v>
+        <v>x5 8</v>
       </c>
       <c r="AC13" t="b">
         <f>$E$9=INT($E$9)</f>
@@ -6020,15 +6051,15 @@
       </c>
       <c r="AF13" s="23">
         <f>AF7</f>
-        <v>1.2463528654218718</v>
+        <v>0.21295975304203327</v>
       </c>
       <c r="AG13">
         <f>1/AF13</f>
-        <v>0.80234099647335022</v>
+        <v>4.695722951005787</v>
       </c>
       <c r="AH13" s="5">
         <f t="shared" ref="AH13:AH15" si="6">AF13/AF$12*100</f>
-        <v>82.29466417370881</v>
+        <v>80.915285620975297</v>
       </c>
     </row>
     <row r="14" spans="1:43">
@@ -6104,7 +6135,7 @@
       </c>
       <c r="AA14" s="21">
         <f>MAX(N22:P33)-MIN(N22:P33)</f>
-        <v>86.087894641279703</v>
+        <v>7.8361878140470598</v>
       </c>
       <c r="AC14" t="b">
         <f>$E$10=INT($E$10)</f>
@@ -6115,15 +6146,15 @@
       </c>
       <c r="AF14" s="23">
         <f>AF8</f>
-        <v>0.25598422423318046</v>
+        <v>4.6744165427919537E-2</v>
       </c>
       <c r="AG14">
         <f>1/AF14</f>
-        <v>3.9064907339332078</v>
+        <v>21.393044262219647</v>
       </c>
       <c r="AH14" s="5">
         <f t="shared" si="6"/>
-        <v>16.902224363167313</v>
+        <v>17.760715077311755</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -6152,23 +6183,23 @@
       </c>
       <c r="L15" s="6">
         <f t="shared" si="2"/>
-        <v>2.4271844660194174E-2</v>
+        <v>1.1210762331838564E-2</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="2"/>
-        <v>1.8796992481203006E-2</v>
+        <v>1.2626262626262626E-2</v>
       </c>
       <c r="N15" s="6">
         <f t="shared" si="2"/>
-        <v>2.0408163265306121E-2</v>
+        <v>1.4534883720930232E-2</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="2"/>
-        <v>2.4390243902439025E-2</v>
+        <v>2.9585798816568046E-2</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="2"/>
-        <v>3.4013605442176874E-2</v>
+        <v>3.0674846625766871E-2</v>
       </c>
       <c r="Q15" s="7">
         <v>0</v>
@@ -6202,15 +6233,15 @@
       </c>
       <c r="AF15" s="23">
         <f>AF9</f>
-        <v>1.2163124831577984E-2</v>
+        <v>3.48461433654664E-3</v>
       </c>
       <c r="AG15">
         <f>1/AF15</f>
-        <v>82.215714616674276</v>
+        <v>286.97580375308644</v>
       </c>
       <c r="AH15" s="5">
         <f t="shared" si="6"/>
-        <v>0.80311146312388704</v>
+        <v>1.3239993017129612</v>
       </c>
     </row>
     <row r="16" spans="1:43">
@@ -6286,7 +6317,7 @@
       </c>
       <c r="AA16" s="21">
         <f>MAX(E5:I16)</f>
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="AC16" t="b">
         <f>$E$12=INT($E$12)</f>
@@ -6297,26 +6328,26 @@
       <c r="B17" s="5"/>
       <c r="E17" s="1">
         <f>SUM(E5:E16)</f>
-        <v>206</v>
+        <v>446</v>
       </c>
       <c r="F17" s="1">
         <f>SUM(F5:F16)</f>
-        <v>266</v>
+        <v>396</v>
       </c>
       <c r="G17" s="1">
         <f>SUM(G5:G16)</f>
-        <v>245</v>
+        <v>344</v>
       </c>
       <c r="H17" s="1">
         <f>SUM(H5:H16)</f>
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="I17" s="1">
         <f>SUM($I$5:I16)</f>
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" ref="L5:P17" si="7">E17/E$17</f>
+        <f t="shared" ref="L17:P17" si="7">E17/E$17</f>
         <v>1</v>
       </c>
       <c r="M17" s="6">
@@ -6363,7 +6394,7 @@
     <row r="19" spans="2:31">
       <c r="AA19">
         <f>_xlfn.STDEV.S(N22:P33)</f>
-        <v>19.987392658442115</v>
+        <v>2.011718026102649</v>
       </c>
       <c r="AC19" t="b">
         <f>$E$15=INT($E$15)</f>
@@ -6383,7 +6414,7 @@
       </c>
       <c r="AA20" s="21">
         <f>SUMSQ(N22:P33)-SUM(N22:P33)*SUM(N22:P33)</f>
-        <v>-26741.642469206701</v>
+        <v>-1341.0320204609552</v>
       </c>
       <c r="AC20" t="b">
         <f>$E$16=INT($E$16)</f>
@@ -6438,7 +6469,7 @@
       </c>
       <c r="AA21">
         <f>_xlfn.VAR.S(N22:P33)</f>
-        <v>399.49586528274574</v>
+        <v>4.0470094165463379</v>
       </c>
       <c r="AC21" t="b">
         <f>$F$5=INT($F$5)</f>
@@ -6452,23 +6483,23 @@
       </c>
       <c r="E22" s="5">
         <f>L5*(1-M5)*100</f>
-        <v>32.119132783414841</v>
+        <v>21.289124428137882</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ref="F22:I33" si="8">E22/(1-M5)*M5*(1-N5)</f>
-        <v>10.391045972370989</v>
+        <v>1.066563012542781</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="8"/>
-        <v>5.8863517703439117</v>
+        <v>5.4150141991177778E-2</v>
       </c>
       <c r="H22" s="9">
         <f t="shared" si="8"/>
-        <v>0.14215339309333935</v>
+        <v>1.0253083335929411E-2</v>
       </c>
       <c r="I22" s="9">
         <f t="shared" si="8"/>
-        <v>5.0054011652584289E-3</v>
+        <v>1.4339976693607565E-3</v>
       </c>
       <c r="K22" s="12">
         <v>0</v>
@@ -6513,7 +6544,7 @@
       </c>
       <c r="AA22" s="21">
         <f>SUM(N22:P33)</f>
-        <v>204.66445843642995</v>
+        <v>39.051754890673251</v>
       </c>
       <c r="AC22" t="b">
         <f>$F$6=INT($F$6)</f>
@@ -6528,23 +6559,23 @@
       </c>
       <c r="E23" s="5">
         <f>L6*(1-M6)*100</f>
-        <v>9.0882546171253367</v>
+        <v>3.3519046971961766</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="8"/>
-        <v>4.8044621162575538</v>
+        <v>1.0665630125427812</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="8"/>
-        <v>0.63768810845392365</v>
+        <v>5.4150141991177791E-2</v>
       </c>
       <c r="H23" s="9">
         <f t="shared" si="8"/>
-        <v>3.0477331539573538E-2</v>
+        <v>9.5360845012490356E-3</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" si="8"/>
-        <v>2.2246227401148569E-3</v>
+        <v>2.1509965040411357E-3</v>
       </c>
       <c r="K23" s="12">
         <f t="shared" ref="K23:K33" si="11">K22+1</f>
@@ -6560,15 +6591,15 @@
       </c>
       <c r="N23" s="16">
         <f t="shared" si="9"/>
-        <v>86.087894641279689</v>
+        <v>7.3102691688090022</v>
       </c>
       <c r="O23" s="8">
         <f t="shared" si="9"/>
-        <v>12.343319273527284</v>
+        <v>3.8621142230058596</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="9"/>
-        <v>3.0032406991550569</v>
+        <v>2.903845280455533</v>
       </c>
       <c r="S23" s="12">
         <f t="shared" ref="S23:S33" si="12">S22+1</f>
@@ -6591,7 +6622,7 @@
       </c>
       <c r="AA23">
         <f>SUMSQ(N22:P33)</f>
-        <v>15145.898077870466</v>
+        <v>184.00753958026689</v>
       </c>
       <c r="AC23" t="b">
         <f>$F$7=INT($F$7)</f>
@@ -6607,23 +6638,23 @@
       </c>
       <c r="E24" s="5">
         <f>L7*(1-M7)*100</f>
-        <v>12.920651142419153</v>
+        <v>4.257824885627576</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="8"/>
-        <v>0.97206559096373757</v>
+        <v>0.16064282411138181</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="8"/>
-        <v>0.63768810845392376</v>
+        <v>5.8045835659607851E-2</v>
       </c>
       <c r="H24" s="9">
         <f t="shared" si="8"/>
-        <v>3.0477331539573545E-2</v>
+        <v>6.8353888906196097E-3</v>
       </c>
       <c r="I24" s="9">
         <f t="shared" si="8"/>
-        <v>2.2246227401148577E-3</v>
+        <v>9.5599844624050473E-4</v>
       </c>
       <c r="K24" s="12">
         <f t="shared" si="11"/>
@@ -6639,15 +6670,15 @@
       </c>
       <c r="N24" s="16">
         <f t="shared" si="9"/>
-        <v>86.087894641279703</v>
+        <v>7.8361878140470598</v>
       </c>
       <c r="O24" s="8">
         <f t="shared" si="9"/>
-        <v>12.343319273527285</v>
+        <v>2.7683325007009421</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" si="9"/>
-        <v>3.0032406991550578</v>
+        <v>1.2905979024246814</v>
       </c>
       <c r="S24" s="12">
         <f t="shared" si="12"/>
@@ -6686,23 +6717,23 @@
       </c>
       <c r="E25" s="5">
         <f t="shared" ref="E25:E30" si="13">L8*(1-M8)*100</f>
-        <v>7.7250164245565367</v>
+        <v>54.355211305883941</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="8"/>
-        <v>0.52095266897181536</v>
+        <v>1.639346852612052</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="8"/>
-        <v>2.4887277271985532E-3</v>
+        <v>5.2241252093647057E-2</v>
       </c>
       <c r="H25" s="9">
         <f t="shared" si="8"/>
-        <v>3.0242767317855833E-3</v>
+        <v>5.9367503511535335E-3</v>
       </c>
       <c r="I25" s="9">
         <f t="shared" si="8"/>
-        <v>9.4508647868299476E-4</v>
+        <v>1.0754982520205676E-3</v>
       </c>
       <c r="K25" s="12">
         <f t="shared" si="11"/>
@@ -6718,15 +6749,15 @@
       </c>
       <c r="N25" s="16">
         <f t="shared" si="9"/>
-        <v>0.22398549544786978</v>
+        <v>4.701712688428235</v>
       </c>
       <c r="O25" s="8">
         <f t="shared" si="9"/>
-        <v>0.6804622646517563</v>
+        <v>1.3357688290095451</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" si="9"/>
-        <v>0.59540448157028669</v>
+        <v>0.67756389877295764</v>
       </c>
       <c r="Q25" s="7"/>
       <c r="S25" s="12">
@@ -6750,7 +6781,7 @@
       </c>
       <c r="AA25" s="21">
         <f>AA23/AA24-(AA22/AA24)^2</f>
-        <v>388.39875791378057</v>
+        <v>3.9345924883089394</v>
       </c>
       <c r="AC25" t="b">
         <f>$F$9=INT($F$9)</f>
@@ -6765,23 +6796,23 @@
       </c>
       <c r="E26" s="5">
         <f t="shared" si="13"/>
-        <v>4.671873859405796</v>
+        <v>1.3317026769941569</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="8"/>
-        <v>0.18026043909059353</v>
+        <v>1.311477482089642</v>
       </c>
       <c r="G26" s="5">
         <f t="shared" si="8"/>
-        <v>1.8531107425156762E-3</v>
+        <v>4.0390551954282837E-2</v>
       </c>
       <c r="H26" s="9">
         <f t="shared" si="8"/>
-        <v>2.0503606254725269E-4</v>
+        <v>5.9797702812343576E-3</v>
       </c>
       <c r="I26" s="9">
         <f t="shared" si="8"/>
-        <v>1.7648673738244536E-4</v>
+        <v>1.0324783219397453E-3</v>
       </c>
       <c r="K26" s="12">
         <f t="shared" si="11"/>
@@ -6797,15 +6828,15 @@
       </c>
       <c r="N26" s="16">
         <f t="shared" si="9"/>
-        <v>0.13342397346112869</v>
+        <v>2.9081197407083641</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" si="9"/>
-        <v>2.7679868443879114E-2</v>
+        <v>0.80726898796663826</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" si="9"/>
-        <v>6.3535225457680325E-2</v>
+        <v>0.37169219589830832</v>
       </c>
       <c r="Q26" s="7"/>
       <c r="S26" s="12">
@@ -6841,23 +6872,23 @@
       </c>
       <c r="E27" s="5">
         <f t="shared" si="13"/>
-        <v>2.3815606978611576</v>
+        <v>2.6090501426824302</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="8"/>
-        <v>4.4692670848907483E-2</v>
+        <v>4.5980716540733234E-2</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="8"/>
-        <v>9.0838761888023328E-4</v>
+        <v>3.050328142380735E-2</v>
       </c>
       <c r="H27" s="9">
         <f t="shared" si="8"/>
-        <v>2.1937252020577062E-5</v>
+        <v>4.3054346024887389E-3</v>
       </c>
       <c r="I27" s="9">
         <f t="shared" si="8"/>
-        <v>7.7243845142876992E-7</v>
+        <v>7.4338439179661689E-4</v>
       </c>
       <c r="K27" s="12">
         <f t="shared" si="11"/>
@@ -6873,15 +6904,15 @@
       </c>
       <c r="N27" s="16">
         <f t="shared" si="9"/>
-        <v>4.9052931419532597E-2</v>
+        <v>1.6471771968855968</v>
       </c>
       <c r="O27" s="8">
         <f t="shared" si="9"/>
-        <v>1.9743526818519356E-3</v>
+        <v>0.38748911422398652</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" si="9"/>
-        <v>1.3903892125717858E-4</v>
+        <v>0.13380919052339105</v>
       </c>
       <c r="Q27" s="7"/>
       <c r="S27" s="12">
@@ -6916,23 +6947,23 @@
       </c>
       <c r="E28" s="5">
         <f t="shared" si="13"/>
-        <v>1.9125483611942475</v>
+        <v>2.6090501426824302</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="8"/>
-        <v>2.8722489798897875E-2</v>
+        <v>7.8688648925378524E-2</v>
       </c>
       <c r="G28" s="5">
         <f t="shared" si="8"/>
-        <v>4.6741993317101291E-4</v>
+        <v>2.7600210502093268E-3</v>
       </c>
       <c r="H28" s="9">
         <f t="shared" si="8"/>
-        <v>9.0487765855694109E-6</v>
+        <v>8.1565787433239865E-5</v>
       </c>
       <c r="I28" s="9">
         <f t="shared" si="8"/>
-        <v>2.5311263176417934E-7</v>
+        <v>2.5811958048493631E-6</v>
       </c>
       <c r="K28" s="12">
         <f t="shared" si="11"/>
@@ -6948,15 +6979,15 @@
       </c>
       <c r="N28" s="16">
         <f t="shared" si="9"/>
-        <v>1.2620338195617349E-2</v>
+        <v>7.4520568355651823E-2</v>
       </c>
       <c r="O28" s="8">
         <f t="shared" si="9"/>
-        <v>4.0719494635062351E-4</v>
+        <v>3.6704604344957939E-3</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" si="9"/>
-        <v>2.2780136858776142E-5</v>
+        <v>2.3230762243644268E-4</v>
       </c>
       <c r="Q28" s="7"/>
       <c r="S28" s="12">
@@ -6990,23 +7021,23 @@
       </c>
       <c r="E29" s="5">
         <f t="shared" si="13"/>
-        <v>1.4398861230746771</v>
+        <v>2.1855324545907502</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="8"/>
-        <v>1.6223439518153415E-2</v>
+        <v>5.4974081202050745E-2</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="8"/>
-        <v>1.9817384293491171E-4</v>
+        <v>1.5972344040563232E-3</v>
       </c>
       <c r="H29" s="9">
         <f t="shared" si="8"/>
-        <v>2.8831110711888549E-6</v>
+        <v>4.720242328312492E-5</v>
       </c>
       <c r="I29" s="9">
         <f t="shared" si="8"/>
-        <v>6.0064813983101139E-8</v>
+        <v>1.4937475722507886E-6</v>
       </c>
       <c r="K29" s="12">
         <f t="shared" si="11"/>
@@ -7022,15 +7053,15 @@
       </c>
       <c r="N29" s="16">
         <f t="shared" si="9"/>
-        <v>3.5671291728284109E-3</v>
+        <v>2.8750219273013817E-2</v>
       </c>
       <c r="O29" s="8">
         <f t="shared" si="9"/>
-        <v>7.7843998922099084E-5</v>
+        <v>1.2744654286443728E-3</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="9"/>
-        <v>3.2434999550874615E-6</v>
+        <v>8.0662368901542581E-5</v>
       </c>
       <c r="Q29" s="7"/>
       <c r="S29" s="12">
@@ -7064,23 +7095,23 @@
       </c>
       <c r="E30" s="5">
         <f t="shared" si="13"/>
-        <v>0.96357398350244527</v>
+        <v>1.1069212302396159</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="8"/>
-        <v>7.2402126775230119E-3</v>
+        <v>1.4031558151122234E-2</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="8"/>
-        <v>5.9008859722459959E-5</v>
+        <v>1.1979258030422425E-4</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="8"/>
-        <v>5.7345830634071874E-7</v>
+        <v>3.540181746234369E-6</v>
       </c>
       <c r="I30" s="9">
         <f t="shared" si="8"/>
-        <v>7.9097697426306045E-9</v>
+        <v>1.1203106791880915E-7</v>
       </c>
       <c r="K30" s="12">
         <f t="shared" si="11"/>
@@ -7096,15 +7127,15 @@
       </c>
       <c r="N30" s="16">
         <f t="shared" si="9"/>
-        <v>2.9504429861229977E-4</v>
+        <v>5.9896290152112129E-4</v>
       </c>
       <c r="O30" s="8">
         <f t="shared" si="9"/>
-        <v>5.1611247570664687E-6</v>
+        <v>3.1861635716109324E-5</v>
       </c>
       <c r="P30" s="8">
         <f t="shared" si="9"/>
-        <v>2.1356378305102632E-7</v>
+        <v>3.0248388338078471E-6</v>
       </c>
       <c r="S30" s="12">
         <f t="shared" si="12"/>
@@ -7210,23 +7241,23 @@
       </c>
       <c r="E32" s="5">
         <f>L15*(1-M15)*100</f>
-        <v>2.3815606978611576</v>
+        <v>1.1069212302396159</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" si="8"/>
-        <v>4.4692670848907483E-2</v>
+        <v>1.3949261622376648E-2</v>
       </c>
       <c r="G32" s="5">
         <f t="shared" si="8"/>
-        <v>9.0838761888023328E-4</v>
+        <v>1.9965430050704038E-4</v>
       </c>
       <c r="H32" s="9">
         <f t="shared" si="8"/>
-        <v>2.1937252020577062E-5</v>
+        <v>5.9003029103906142E-6</v>
       </c>
       <c r="I32" s="9">
         <f t="shared" si="8"/>
-        <v>7.7243845142876992E-7</v>
+        <v>1.8671844653134855E-7</v>
       </c>
       <c r="K32" s="12">
         <f t="shared" si="11"/>
@@ -7242,15 +7273,15 @@
       </c>
       <c r="N32" s="16">
         <f t="shared" si="9"/>
-        <v>2.7251628566406999E-3</v>
+        <v>5.9896290152112119E-4</v>
       </c>
       <c r="O32" s="8">
         <f t="shared" si="9"/>
-        <v>1.5356076414403943E-4</v>
+        <v>4.1302120372734301E-5</v>
       </c>
       <c r="P32" s="8">
         <f t="shared" si="9"/>
-        <v>1.3903892125717859E-5</v>
+        <v>3.3609320375642738E-6</v>
       </c>
       <c r="S32" s="12">
         <f t="shared" si="12"/>

</xml_diff>